<commit_message>
Updated during drafting the design specification
</commit_message>
<xml_diff>
--- a/docs/Mockups.xlsx
+++ b/docs/Mockups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="14" r:id="rId1"/>
@@ -1514,14 +1514,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1529,7 +1529,13 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1538,29 +1544,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1569,6 +1566,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1584,18 +1584,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1616,6 +1604,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1624,6 +1621,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1723,18 +1723,18 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>58343</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>48057</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>217967</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1747,8 +1747,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1771650" y="942975"/>
-          <a:ext cx="8545118" cy="3096057"/>
+          <a:off x="1771650" y="1133476"/>
+          <a:ext cx="9476267" cy="3543300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3143,12 +3143,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -3503,18 +3503,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="B30:E30"/>
@@ -3531,6 +3519,18 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3628,12 +3628,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -3716,11 +3716,11 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="128">
+      <c r="L8" s="129">
         <v>45336</v>
       </c>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="129"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
         <v>127</v>
@@ -3770,11 +3770,11 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="128">
+      <c r="L9" s="129">
         <v>45324</v>
       </c>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="129"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
         <v>128</v>
@@ -3826,11 +3826,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="128">
+      <c r="L10" s="129">
         <v>45241</v>
       </c>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="129"/>
       <c r="O10" s="10"/>
       <c r="P10" s="9" t="s">
         <v>127</v>
@@ -3880,11 +3880,11 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="128">
+      <c r="L11" s="129">
         <v>45281</v>
       </c>
-      <c r="M11" s="128"/>
-      <c r="N11" s="128"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
         <v>129</v>
@@ -3934,11 +3934,11 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="128">
+      <c r="L12" s="129">
         <v>45220</v>
       </c>
-      <c r="M12" s="128"/>
-      <c r="N12" s="128"/>
+      <c r="M12" s="129"/>
+      <c r="N12" s="129"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
         <v>130</v>
@@ -4737,21 +4737,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -4768,6 +4753,21 @@
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4882,12 +4882,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -5462,17 +5462,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B24:E24"/>
@@ -5489,6 +5478,17 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5586,25 +5586,25 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="N5" s="139" t="s">
+      <c r="N5" s="138" t="s">
         <v>185</v>
       </c>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="141"/>
+      <c r="O5" s="139"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="140"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121" t="s">
@@ -5680,17 +5680,17 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="128">
+      <c r="K8" s="129">
         <v>45353</v>
       </c>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="131">
+      <c r="O8" s="128">
         <v>10</v>
       </c>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="128"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10" t="s">
         <v>127</v>
@@ -5706,9 +5706,9 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
       <c r="AB8" s="10"/>
-      <c r="AC8" s="138"/>
-      <c r="AD8" s="138"/>
-      <c r="AE8" s="138"/>
+      <c r="AC8" s="141"/>
+      <c r="AD8" s="141"/>
+      <c r="AE8" s="141"/>
       <c r="AF8" s="86"/>
       <c r="AG8" s="10" t="s">
         <v>175</v>
@@ -5736,17 +5736,17 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="128">
+      <c r="K9" s="129">
         <v>45353</v>
       </c>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="131">
+      <c r="O9" s="128">
         <v>10</v>
       </c>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="128"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10" t="s">
         <v>127</v>
@@ -5762,9 +5762,9 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
-      <c r="AC9" s="138"/>
-      <c r="AD9" s="138"/>
-      <c r="AE9" s="138"/>
+      <c r="AC9" s="141"/>
+      <c r="AD9" s="141"/>
+      <c r="AE9" s="141"/>
       <c r="AF9" s="86"/>
       <c r="AG9" s="10" t="s">
         <v>175</v>
@@ -5788,13 +5788,13 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="128"/>
+      <c r="Q10" s="128"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5806,9 +5806,9 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
-      <c r="AC10" s="138"/>
-      <c r="AD10" s="138"/>
-      <c r="AE10" s="138"/>
+      <c r="AC10" s="141"/>
+      <c r="AD10" s="141"/>
+      <c r="AE10" s="141"/>
       <c r="AF10" s="86"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="86"/>
@@ -5834,17 +5834,17 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="128">
+      <c r="K11" s="129">
         <v>45354</v>
       </c>
-      <c r="L11" s="128"/>
-      <c r="M11" s="128"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="131">
+      <c r="O11" s="128">
         <v>5</v>
       </c>
-      <c r="P11" s="131"/>
-      <c r="Q11" s="131"/>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="128"/>
       <c r="R11" s="10"/>
       <c r="S11" s="9" t="s">
         <v>130</v>
@@ -5860,9 +5860,9 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
-      <c r="AC11" s="138"/>
-      <c r="AD11" s="138"/>
-      <c r="AE11" s="138"/>
+      <c r="AC11" s="141"/>
+      <c r="AD11" s="141"/>
+      <c r="AE11" s="141"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="9" t="s">
         <v>176</v>
@@ -5888,17 +5888,17 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="128">
+      <c r="K12" s="129">
         <v>45355</v>
       </c>
-      <c r="L12" s="128"/>
-      <c r="M12" s="128"/>
+      <c r="L12" s="129"/>
+      <c r="M12" s="129"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="131">
+      <c r="O12" s="128">
         <v>10</v>
       </c>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="131"/>
+      <c r="P12" s="128"/>
+      <c r="Q12" s="128"/>
       <c r="R12" s="10"/>
       <c r="S12" s="9" t="s">
         <v>128</v>
@@ -5944,17 +5944,17 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="128">
+      <c r="K13" s="129">
         <v>45356</v>
       </c>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="131">
+      <c r="O13" s="128">
         <v>20</v>
       </c>
-      <c r="P13" s="131"/>
-      <c r="Q13" s="131"/>
+      <c r="P13" s="128"/>
+      <c r="Q13" s="128"/>
       <c r="R13" s="10"/>
       <c r="S13" s="9" t="s">
         <v>129</v>
@@ -6187,26 +6187,26 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="131">
+      <c r="M21" s="128">
         <v>30</v>
       </c>
-      <c r="N21" s="131"/>
-      <c r="O21" s="131"/>
+      <c r="N21" s="128"/>
+      <c r="O21" s="128"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="131">
+      <c r="Q21" s="128">
         <v>35</v>
       </c>
-      <c r="R21" s="131"/>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
+      <c r="R21" s="128"/>
+      <c r="S21" s="128"/>
+      <c r="T21" s="128"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="131">
+      <c r="V21" s="128">
         <f>M21-Q21</f>
         <v>-5</v>
       </c>
-      <c r="W21" s="131"/>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="131"/>
+      <c r="W21" s="128"/>
+      <c r="X21" s="128"/>
+      <c r="Y21" s="128"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="44"/>
     </row>
@@ -6223,26 +6223,26 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="131">
+      <c r="M22" s="128">
         <v>20</v>
       </c>
-      <c r="N22" s="131"/>
-      <c r="O22" s="131"/>
+      <c r="N22" s="128"/>
+      <c r="O22" s="128"/>
       <c r="P22" s="10"/>
-      <c r="Q22" s="131">
+      <c r="Q22" s="128">
         <v>10</v>
       </c>
-      <c r="R22" s="131"/>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
+      <c r="R22" s="128"/>
+      <c r="S22" s="128"/>
+      <c r="T22" s="128"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="131">
+      <c r="V22" s="128">
         <f>M22-Q22</f>
         <v>10</v>
       </c>
-      <c r="W22" s="131"/>
-      <c r="X22" s="131"/>
-      <c r="Y22" s="131"/>
+      <c r="W22" s="128"/>
+      <c r="X22" s="128"/>
+      <c r="Y22" s="128"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="44"/>
     </row>
@@ -6259,26 +6259,26 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="131">
+      <c r="M23" s="128">
         <v>5</v>
       </c>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
+      <c r="N23" s="128"/>
+      <c r="O23" s="128"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="131">
+      <c r="Q23" s="128">
         <v>10</v>
       </c>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
+      <c r="R23" s="128"/>
+      <c r="S23" s="128"/>
+      <c r="T23" s="128"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="131">
+      <c r="V23" s="128">
         <f>M23-Q23</f>
         <v>-5</v>
       </c>
-      <c r="W23" s="131"/>
-      <c r="X23" s="131"/>
-      <c r="Y23" s="131"/>
+      <c r="W23" s="128"/>
+      <c r="X23" s="128"/>
+      <c r="Y23" s="128"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="44"/>
     </row>
@@ -6295,26 +6295,26 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="131">
+      <c r="M24" s="128">
         <v>10</v>
       </c>
-      <c r="N24" s="131"/>
-      <c r="O24" s="131"/>
+      <c r="N24" s="128"/>
+      <c r="O24" s="128"/>
       <c r="P24" s="10"/>
-      <c r="Q24" s="131">
+      <c r="Q24" s="128">
         <v>10</v>
       </c>
-      <c r="R24" s="131"/>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
+      <c r="R24" s="128"/>
+      <c r="S24" s="128"/>
+      <c r="T24" s="128"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="131">
+      <c r="V24" s="128">
         <f>M24-Q24</f>
         <v>0</v>
       </c>
-      <c r="W24" s="131"/>
-      <c r="X24" s="131"/>
-      <c r="Y24" s="131"/>
+      <c r="W24" s="128"/>
+      <c r="X24" s="128"/>
+      <c r="Y24" s="128"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="44"/>
     </row>
@@ -6380,15 +6380,36 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="Q21:T21"/>
-    <mergeCell ref="Q22:T22"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="AC11:AE11"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="AC10:AE10"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="M21:O21"/>
@@ -6405,36 +6426,15 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="AC11:AE11"/>
-    <mergeCell ref="AC9:AE9"/>
-    <mergeCell ref="AC10:AE10"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V23:Y23"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="Q22:T22"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q24:T24"/>
   </mergeCells>
   <conditionalFormatting sqref="V21:Y24">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -6559,12 +6559,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -7083,20 +7083,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="H8:R8"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -7113,6 +7099,20 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7517,10 +7517,10 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="44"/>
-      <c r="J46" s="139" t="s">
+      <c r="J46" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="K46" s="141"/>
+      <c r="K46" s="140"/>
       <c r="M46" s="144"/>
       <c r="N46" s="144"/>
       <c r="O46" s="144"/>
@@ -7846,7 +7846,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AS31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
@@ -7939,46 +7939,46 @@
       <c r="C5" s="121"/>
       <c r="D5" s="121"/>
       <c r="E5" s="146"/>
-      <c r="G5" s="147" t="s">
+      <c r="G5" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="147"/>
-      <c r="AI5" s="147"/>
-      <c r="AJ5" s="147"/>
-      <c r="AK5" s="147"/>
-      <c r="AL5" s="147"/>
-      <c r="AM5" s="147"/>
-      <c r="AN5" s="147"/>
-      <c r="AO5" s="147"/>
-      <c r="AP5" s="147"/>
-      <c r="AQ5" s="147"/>
-      <c r="AR5" s="147"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="159"/>
+      <c r="AK5" s="159"/>
+      <c r="AL5" s="159"/>
+      <c r="AM5" s="159"/>
+      <c r="AN5" s="159"/>
+      <c r="AO5" s="159"/>
+      <c r="AP5" s="159"/>
+      <c r="AQ5" s="159"/>
+      <c r="AR5" s="159"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -8095,13 +8095,13 @@
       <c r="C8" s="121"/>
       <c r="D8" s="121"/>
       <c r="E8" s="146"/>
-      <c r="G8" s="157" t="s">
+      <c r="G8" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="158"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="159"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="157"/>
+      <c r="K8" s="158"/>
       <c r="L8" s="25" t="s">
         <v>25</v>
       </c>
@@ -8210,13 +8210,13 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="146"/>
-      <c r="G9" s="148" t="s">
+      <c r="G9" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="149"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="149"/>
-      <c r="K9" s="150"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="155"/>
       <c r="L9" s="24">
         <f t="shared" ref="L9:M12" si="0">SUM(M9:AQ9)</f>
         <v>610</v>
@@ -8324,13 +8324,13 @@
       <c r="C10" s="121"/>
       <c r="D10" s="121"/>
       <c r="E10" s="146"/>
-      <c r="G10" s="148" t="s">
+      <c r="G10" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="149"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="150"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="155"/>
       <c r="L10" s="24">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -8380,13 +8380,13 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="146"/>
-      <c r="G11" s="148" t="s">
+      <c r="G11" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="149"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="149"/>
-      <c r="K11" s="150"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="155"/>
       <c r="L11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8432,13 +8432,13 @@
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
       <c r="E12" s="146"/>
-      <c r="G12" s="148" t="s">
+      <c r="G12" s="153" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="150"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="155"/>
       <c r="L12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8484,13 +8484,13 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="146"/>
-      <c r="G13" s="148" t="s">
+      <c r="G13" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="149"/>
-      <c r="K13" s="150"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
+      <c r="K13" s="155"/>
       <c r="L13" s="24">
         <v>500</v>
       </c>
@@ -8541,13 +8541,13 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="146"/>
-      <c r="G14" s="148" t="s">
+      <c r="G14" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="149"/>
-      <c r="I14" s="149"/>
-      <c r="J14" s="149"/>
-      <c r="K14" s="150"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="155"/>
       <c r="L14" s="24">
         <f>SUM(M14:AQ14)</f>
         <v>246</v>
@@ -8595,13 +8595,13 @@
       <c r="C15" s="121"/>
       <c r="D15" s="121"/>
       <c r="E15" s="146"/>
-      <c r="G15" s="148" t="s">
+      <c r="G15" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="149"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="149"/>
-      <c r="K15" s="150"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="155"/>
       <c r="L15" s="24">
         <f>SUM(M15:AQ15)</f>
         <v>220</v>
@@ -8649,13 +8649,13 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="G16" s="151" t="s">
+      <c r="G16" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="152"/>
-      <c r="I16" s="152"/>
-      <c r="J16" s="152"/>
-      <c r="K16" s="153"/>
+      <c r="H16" s="148"/>
+      <c r="I16" s="148"/>
+      <c r="J16" s="148"/>
+      <c r="K16" s="149"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="11"/>
@@ -8695,13 +8695,13 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="146"/>
-      <c r="G17" s="154" t="s">
+      <c r="G17" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="155"/>
-      <c r="I17" s="155"/>
-      <c r="J17" s="155"/>
-      <c r="K17" s="156"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="26">
         <f>SUM(L9:L16)</f>
         <v>1976</v>
@@ -8863,46 +8863,46 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="146"/>
-      <c r="G21" s="147" t="s">
+      <c r="G21" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="147"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="147"/>
-      <c r="K21" s="147"/>
-      <c r="L21" s="147"/>
-      <c r="M21" s="147"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="147"/>
-      <c r="P21" s="147"/>
-      <c r="Q21" s="147"/>
-      <c r="R21" s="147"/>
-      <c r="S21" s="147"/>
-      <c r="T21" s="147"/>
-      <c r="U21" s="147"/>
-      <c r="V21" s="147"/>
-      <c r="W21" s="147"/>
-      <c r="X21" s="147"/>
-      <c r="Y21" s="147"/>
-      <c r="Z21" s="147"/>
-      <c r="AA21" s="147"/>
-      <c r="AB21" s="147"/>
-      <c r="AC21" s="147"/>
-      <c r="AD21" s="147"/>
-      <c r="AE21" s="147"/>
-      <c r="AF21" s="147"/>
-      <c r="AG21" s="147"/>
-      <c r="AH21" s="147"/>
-      <c r="AI21" s="147"/>
-      <c r="AJ21" s="147"/>
-      <c r="AK21" s="147"/>
-      <c r="AL21" s="147"/>
-      <c r="AM21" s="147"/>
-      <c r="AN21" s="147"/>
-      <c r="AO21" s="147"/>
-      <c r="AP21" s="147"/>
-      <c r="AQ21" s="147"/>
-      <c r="AR21" s="147"/>
+      <c r="H21" s="159"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="159"/>
+      <c r="K21" s="159"/>
+      <c r="L21" s="159"/>
+      <c r="M21" s="159"/>
+      <c r="N21" s="159"/>
+      <c r="O21" s="159"/>
+      <c r="P21" s="159"/>
+      <c r="Q21" s="159"/>
+      <c r="R21" s="159"/>
+      <c r="S21" s="159"/>
+      <c r="T21" s="159"/>
+      <c r="U21" s="159"/>
+      <c r="V21" s="159"/>
+      <c r="W21" s="159"/>
+      <c r="X21" s="159"/>
+      <c r="Y21" s="159"/>
+      <c r="Z21" s="159"/>
+      <c r="AA21" s="159"/>
+      <c r="AB21" s="159"/>
+      <c r="AC21" s="159"/>
+      <c r="AD21" s="159"/>
+      <c r="AE21" s="159"/>
+      <c r="AF21" s="159"/>
+      <c r="AG21" s="159"/>
+      <c r="AH21" s="159"/>
+      <c r="AI21" s="159"/>
+      <c r="AJ21" s="159"/>
+      <c r="AK21" s="159"/>
+      <c r="AL21" s="159"/>
+      <c r="AM21" s="159"/>
+      <c r="AN21" s="159"/>
+      <c r="AO21" s="159"/>
+      <c r="AP21" s="159"/>
+      <c r="AQ21" s="159"/>
+      <c r="AR21" s="159"/>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B22" s="121"/>
@@ -9015,13 +9015,13 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="146"/>
-      <c r="G24" s="157" t="s">
+      <c r="G24" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="158"/>
-      <c r="K24" s="159"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="158"/>
       <c r="L24" s="25" t="s">
         <v>25</v>
       </c>
@@ -9127,13 +9127,13 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="146"/>
-      <c r="G25" s="148" t="s">
+      <c r="G25" s="153" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="149"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="150"/>
+      <c r="H25" s="154"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="154"/>
+      <c r="K25" s="155"/>
       <c r="L25" s="24">
         <f>SUM(M25:AQ25)</f>
         <v>610</v>
@@ -9241,13 +9241,13 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="146"/>
-      <c r="G26" s="148" t="s">
+      <c r="G26" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="150"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="154"/>
+      <c r="K26" s="155"/>
       <c r="L26" s="24">
         <f>SUM(M26:AQ26)</f>
         <v>400</v>
@@ -9297,13 +9297,13 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="146"/>
-      <c r="G27" s="151" t="s">
+      <c r="G27" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="152"/>
-      <c r="K27" s="153"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
+      <c r="K27" s="149"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="11"/>
@@ -9343,13 +9343,13 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="146"/>
-      <c r="G28" s="154" t="s">
+      <c r="G28" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="155"/>
-      <c r="I28" s="155"/>
-      <c r="J28" s="155"/>
-      <c r="K28" s="156"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="151"/>
+      <c r="K28" s="152"/>
       <c r="L28" s="26">
         <f>SUM(L25:L27)</f>
         <v>1010</v>
@@ -9507,24 +9507,15 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G21:AR21"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="G5:AR5"/>
     <mergeCell ref="G9:K9"/>
@@ -9541,15 +9532,24 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G21:AR21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:L16">
     <cfRule type="dataBar" priority="2">
@@ -9708,43 +9708,43 @@
       <c r="G5" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="147"/>
-      <c r="AI5" s="147"/>
-      <c r="AJ5" s="147"/>
-      <c r="AK5" s="147"/>
-      <c r="AL5" s="147"/>
-      <c r="AM5" s="147"/>
-      <c r="AN5" s="147"/>
-      <c r="AO5" s="147"/>
-      <c r="AP5" s="147"/>
-      <c r="AQ5" s="147"/>
-      <c r="AR5" s="147"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="159"/>
+      <c r="AK5" s="159"/>
+      <c r="AL5" s="159"/>
+      <c r="AM5" s="159"/>
+      <c r="AN5" s="159"/>
+      <c r="AO5" s="159"/>
+      <c r="AP5" s="159"/>
+      <c r="AQ5" s="159"/>
+      <c r="AR5" s="159"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -9753,11 +9753,11 @@
       <c r="E6" s="146"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="161"/>
       <c r="G7" s="40" t="s">
         <v>28</v>
@@ -10216,23 +10216,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:AR5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:AR5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11306,24 +11306,24 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="G5" s="120" t="s">
         <v>168</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="123" t="s">
+      <c r="K5" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
@@ -11500,20 +11500,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B31:E31"/>
@@ -11530,6 +11516,20 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:N5">
@@ -11545,8 +11545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11643,12 +11643,12 @@
       <c r="E5" s="122"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -11798,12 +11798,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -11816,14 +11818,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11922,12 +11922,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -12846,12 +12846,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -12864,14 +12866,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12983,12 +12983,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -13229,12 +13229,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -13247,14 +13249,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13352,12 +13352,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -13387,11 +13387,11 @@
       <c r="K7" s="68"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="130" t="s">
+      <c r="N7" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
       <c r="Q7" s="68"/>
       <c r="R7" s="68" t="s">
         <v>25</v>
@@ -13428,17 +13428,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="128">
+      <c r="N8" s="129">
         <v>45334</v>
       </c>
-      <c r="O8" s="128"/>
-      <c r="P8" s="128"/>
+      <c r="O8" s="129"/>
+      <c r="P8" s="129"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="131">
+      <c r="R8" s="128">
         <v>500</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
+      <c r="S8" s="128"/>
+      <c r="T8" s="128"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -13460,17 +13460,17 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="128">
+      <c r="N9" s="129">
         <v>45334</v>
       </c>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
+      <c r="O9" s="129"/>
+      <c r="P9" s="129"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="131">
+      <c r="R9" s="128">
         <v>501</v>
       </c>
-      <c r="S9" s="131"/>
-      <c r="T9" s="131"/>
+      <c r="S9" s="128"/>
+      <c r="T9" s="128"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -13492,17 +13492,17 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="128">
+      <c r="N10" s="129">
         <v>45334</v>
       </c>
-      <c r="O10" s="128"/>
-      <c r="P10" s="128"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="129"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="131">
+      <c r="R10" s="128">
         <v>502</v>
       </c>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
+      <c r="S10" s="128"/>
+      <c r="T10" s="128"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -13524,17 +13524,17 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="128">
+      <c r="N11" s="129">
         <v>45334</v>
       </c>
-      <c r="O11" s="128"/>
-      <c r="P11" s="128"/>
+      <c r="O11" s="129"/>
+      <c r="P11" s="129"/>
       <c r="Q11" s="10"/>
-      <c r="R11" s="131">
+      <c r="R11" s="128">
         <v>503</v>
       </c>
-      <c r="S11" s="131"/>
-      <c r="T11" s="131"/>
+      <c r="S11" s="128"/>
+      <c r="T11" s="128"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -13556,17 +13556,17 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="128">
+      <c r="N12" s="129">
         <v>45334</v>
       </c>
-      <c r="O12" s="128"/>
-      <c r="P12" s="128"/>
+      <c r="O12" s="129"/>
+      <c r="P12" s="129"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="131">
+      <c r="R12" s="128">
         <v>504</v>
       </c>
-      <c r="S12" s="131"/>
-      <c r="T12" s="131"/>
+      <c r="S12" s="128"/>
+      <c r="T12" s="128"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -13588,17 +13588,17 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="128">
+      <c r="N13" s="129">
         <v>45334</v>
       </c>
-      <c r="O13" s="128"/>
-      <c r="P13" s="128"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
       <c r="Q13" s="10"/>
-      <c r="R13" s="131">
+      <c r="R13" s="128">
         <v>505</v>
       </c>
-      <c r="S13" s="131"/>
-      <c r="T13" s="131"/>
+      <c r="S13" s="128"/>
+      <c r="T13" s="128"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -13620,17 +13620,17 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="128">
+      <c r="N14" s="129">
         <v>45334</v>
       </c>
-      <c r="O14" s="128"/>
-      <c r="P14" s="128"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="129"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="131">
+      <c r="R14" s="128">
         <v>506</v>
       </c>
-      <c r="S14" s="131"/>
-      <c r="T14" s="131"/>
+      <c r="S14" s="128"/>
+      <c r="T14" s="128"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -13652,17 +13652,17 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="128">
+      <c r="N15" s="129">
         <v>45334</v>
       </c>
-      <c r="O15" s="128"/>
-      <c r="P15" s="128"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="129"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="131">
+      <c r="R15" s="128">
         <v>507</v>
       </c>
-      <c r="S15" s="131"/>
-      <c r="T15" s="131"/>
+      <c r="S15" s="128"/>
+      <c r="T15" s="128"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
@@ -13684,17 +13684,17 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="128">
+      <c r="N16" s="129">
         <v>45334</v>
       </c>
-      <c r="O16" s="128"/>
-      <c r="P16" s="128"/>
+      <c r="O16" s="129"/>
+      <c r="P16" s="129"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="131">
+      <c r="R16" s="128">
         <v>508</v>
       </c>
-      <c r="S16" s="131"/>
-      <c r="T16" s="131"/>
+      <c r="S16" s="128"/>
+      <c r="T16" s="128"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -13717,17 +13717,17 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="128">
+      <c r="N17" s="129">
         <v>45334</v>
       </c>
-      <c r="O17" s="128"/>
-      <c r="P17" s="128"/>
+      <c r="O17" s="129"/>
+      <c r="P17" s="129"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="131">
+      <c r="R17" s="128">
         <v>509</v>
       </c>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
+      <c r="S17" s="128"/>
+      <c r="T17" s="128"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -13749,17 +13749,17 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="128">
+      <c r="N18" s="129">
         <v>45334</v>
       </c>
-      <c r="O18" s="128"/>
-      <c r="P18" s="128"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="129"/>
       <c r="Q18" s="10"/>
-      <c r="R18" s="131">
+      <c r="R18" s="128">
         <v>510</v>
       </c>
-      <c r="S18" s="131"/>
-      <c r="T18" s="131"/>
+      <c r="S18" s="128"/>
+      <c r="T18" s="128"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
@@ -13781,17 +13781,17 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="128">
+      <c r="N19" s="129">
         <v>45334</v>
       </c>
-      <c r="O19" s="128"/>
-      <c r="P19" s="128"/>
+      <c r="O19" s="129"/>
+      <c r="P19" s="129"/>
       <c r="Q19" s="10"/>
-      <c r="R19" s="131">
+      <c r="R19" s="128">
         <v>511</v>
       </c>
-      <c r="S19" s="131"/>
-      <c r="T19" s="131"/>
+      <c r="S19" s="128"/>
+      <c r="T19" s="128"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -13813,17 +13813,17 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="128">
+      <c r="N20" s="129">
         <v>45334</v>
       </c>
-      <c r="O20" s="128"/>
-      <c r="P20" s="128"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="129"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="131">
+      <c r="R20" s="128">
         <v>512</v>
       </c>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
+      <c r="S20" s="128"/>
+      <c r="T20" s="128"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
@@ -13845,17 +13845,17 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="128">
+      <c r="N21" s="129">
         <v>45292</v>
       </c>
-      <c r="O21" s="128"/>
-      <c r="P21" s="128"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="129"/>
       <c r="Q21" s="10"/>
-      <c r="R21" s="131">
+      <c r="R21" s="128">
         <v>513</v>
       </c>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
+      <c r="S21" s="128"/>
+      <c r="T21" s="128"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -13877,17 +13877,17 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="128">
+      <c r="N22" s="129">
         <v>45292</v>
       </c>
-      <c r="O22" s="128"/>
-      <c r="P22" s="128"/>
+      <c r="O22" s="129"/>
+      <c r="P22" s="129"/>
       <c r="Q22" s="10"/>
-      <c r="R22" s="131">
+      <c r="R22" s="128">
         <v>514</v>
       </c>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
+      <c r="S22" s="128"/>
+      <c r="T22" s="128"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
@@ -13909,17 +13909,17 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="128">
+      <c r="N23" s="129">
         <v>45292</v>
       </c>
-      <c r="O23" s="128"/>
-      <c r="P23" s="128"/>
+      <c r="O23" s="129"/>
+      <c r="P23" s="129"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="131">
+      <c r="R23" s="128">
         <v>515</v>
       </c>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
+      <c r="S23" s="128"/>
+      <c r="T23" s="128"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -13941,17 +13941,17 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="128">
+      <c r="N24" s="129">
         <v>45292</v>
       </c>
-      <c r="O24" s="128"/>
-      <c r="P24" s="128"/>
+      <c r="O24" s="129"/>
+      <c r="P24" s="129"/>
       <c r="Q24" s="10"/>
-      <c r="R24" s="131">
+      <c r="R24" s="128">
         <v>516</v>
       </c>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
+      <c r="S24" s="128"/>
+      <c r="T24" s="128"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -13973,17 +13973,17 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="128">
+      <c r="N25" s="129">
         <v>45292</v>
       </c>
-      <c r="O25" s="128"/>
-      <c r="P25" s="128"/>
+      <c r="O25" s="129"/>
+      <c r="P25" s="129"/>
       <c r="Q25" s="10"/>
-      <c r="R25" s="131">
+      <c r="R25" s="128">
         <v>517</v>
       </c>
-      <c r="S25" s="131"/>
-      <c r="T25" s="131"/>
+      <c r="S25" s="128"/>
+      <c r="T25" s="128"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -14005,17 +14005,17 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="128">
+      <c r="N26" s="129">
         <v>45292</v>
       </c>
-      <c r="O26" s="128"/>
-      <c r="P26" s="128"/>
+      <c r="O26" s="129"/>
+      <c r="P26" s="129"/>
       <c r="Q26" s="10"/>
-      <c r="R26" s="131">
+      <c r="R26" s="128">
         <v>518</v>
       </c>
-      <c r="S26" s="131"/>
-      <c r="T26" s="131"/>
+      <c r="S26" s="128"/>
+      <c r="T26" s="128"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -14037,17 +14037,17 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="128">
+      <c r="N27" s="129">
         <v>45292</v>
       </c>
-      <c r="O27" s="128"/>
-      <c r="P27" s="128"/>
+      <c r="O27" s="129"/>
+      <c r="P27" s="129"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="131">
+      <c r="R27" s="128">
         <v>519</v>
       </c>
-      <c r="S27" s="131"/>
-      <c r="T27" s="131"/>
+      <c r="S27" s="128"/>
+      <c r="T27" s="128"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
@@ -14069,17 +14069,17 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="128">
+      <c r="N28" s="129">
         <v>45292</v>
       </c>
-      <c r="O28" s="128"/>
-      <c r="P28" s="128"/>
+      <c r="O28" s="129"/>
+      <c r="P28" s="129"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="131">
+      <c r="R28" s="128">
         <v>520</v>
       </c>
-      <c r="S28" s="131"/>
-      <c r="T28" s="131"/>
+      <c r="S28" s="128"/>
+      <c r="T28" s="128"/>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
@@ -14101,17 +14101,17 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="128">
+      <c r="N29" s="129">
         <v>45292</v>
       </c>
-      <c r="O29" s="128"/>
-      <c r="P29" s="128"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="131">
+      <c r="R29" s="128">
         <v>521</v>
       </c>
-      <c r="S29" s="131"/>
-      <c r="T29" s="131"/>
+      <c r="S29" s="128"/>
+      <c r="T29" s="128"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
@@ -14133,17 +14133,17 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="129">
+      <c r="N30" s="131">
         <v>45292</v>
       </c>
-      <c r="O30" s="129"/>
-      <c r="P30" s="129"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="132">
+      <c r="R30" s="130">
         <v>522</v>
       </c>
-      <c r="S30" s="132"/>
-      <c r="T30" s="132"/>
+      <c r="S30" s="130"/>
+      <c r="T30" s="130"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -14153,24 +14153,45 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R21:T21"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="R8:T8"/>
@@ -14187,45 +14208,24 @@
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14337,12 +14337,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -14631,18 +14631,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H12:J12"/>
@@ -14659,6 +14647,18 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14758,12 +14758,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -14838,11 +14838,11 @@
       <c r="C8" s="126"/>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
-      <c r="G8" s="136" t="s">
+      <c r="G8" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="128"/>
-      <c r="I8" s="128"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10" t="s">
         <v>12</v>
@@ -14851,17 +14851,17 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="128">
+      <c r="P8" s="129">
         <v>45330</v>
       </c>
-      <c r="Q8" s="128"/>
-      <c r="R8" s="128"/>
+      <c r="Q8" s="129"/>
+      <c r="R8" s="129"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="131">
+      <c r="T8" s="128">
         <v>125</v>
       </c>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10" t="str">
@@ -14892,11 +14892,11 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="122"/>
-      <c r="G9" s="136" t="s">
+      <c r="G9" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="128"/>
-      <c r="I9" s="128"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>84</v>
@@ -14905,17 +14905,17 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="128">
+      <c r="P9" s="129">
         <v>45329</v>
       </c>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="128"/>
+      <c r="Q9" s="129"/>
+      <c r="R9" s="129"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="131">
+      <c r="T9" s="128">
         <v>120</v>
       </c>
-      <c r="U9" s="131"/>
-      <c r="V9" s="131"/>
+      <c r="U9" s="128"/>
+      <c r="V9" s="128"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10" t="str">
@@ -14948,11 +14948,11 @@
       <c r="C10" s="126"/>
       <c r="D10" s="126"/>
       <c r="E10" s="127"/>
-      <c r="G10" s="136" t="s">
+      <c r="G10" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
         <v>69</v>
@@ -14961,17 +14961,17 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="128">
+      <c r="P10" s="129">
         <v>45328</v>
       </c>
-      <c r="Q10" s="128"/>
-      <c r="R10" s="128"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="129"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="131">
+      <c r="T10" s="128">
         <v>127</v>
       </c>
-      <c r="U10" s="131"/>
-      <c r="V10" s="131"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10" t="str">
@@ -15002,11 +15002,11 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="122"/>
-      <c r="G11" s="136" t="s">
+      <c r="G11" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
         <v>70</v>
@@ -15015,17 +15015,17 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="128">
+      <c r="P11" s="129">
         <v>45327</v>
       </c>
-      <c r="Q11" s="128"/>
-      <c r="R11" s="128"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="131">
+      <c r="T11" s="128">
         <v>128</v>
       </c>
-      <c r="U11" s="131"/>
-      <c r="V11" s="131"/>
+      <c r="U11" s="128"/>
+      <c r="V11" s="128"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10" t="str">
@@ -15056,11 +15056,11 @@
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
       <c r="E12" s="127"/>
-      <c r="G12" s="136" t="s">
+      <c r="G12" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10" t="s">
         <v>71</v>
@@ -15069,17 +15069,17 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="128">
+      <c r="P12" s="129">
         <v>45326</v>
       </c>
-      <c r="Q12" s="128"/>
-      <c r="R12" s="128"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="129"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="131">
+      <c r="T12" s="128">
         <v>129</v>
       </c>
-      <c r="U12" s="131"/>
-      <c r="V12" s="131"/>
+      <c r="U12" s="128"/>
+      <c r="V12" s="128"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10" t="str">
@@ -15110,11 +15110,11 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="122"/>
-      <c r="G13" s="136" t="s">
+      <c r="G13" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
         <v>72</v>
@@ -15123,17 +15123,17 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="128">
+      <c r="P13" s="129">
         <v>45325</v>
       </c>
-      <c r="Q13" s="128"/>
-      <c r="R13" s="128"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="129"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="131">
+      <c r="T13" s="128">
         <v>130</v>
       </c>
-      <c r="U13" s="131"/>
-      <c r="V13" s="131"/>
+      <c r="U13" s="128"/>
+      <c r="V13" s="128"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10" t="str">
@@ -15164,11 +15164,11 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="122"/>
-      <c r="G14" s="136" t="s">
+      <c r="G14" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
         <v>73</v>
@@ -15177,17 +15177,17 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="128">
+      <c r="P14" s="129">
         <v>45324</v>
       </c>
-      <c r="Q14" s="128"/>
-      <c r="R14" s="128"/>
+      <c r="Q14" s="129"/>
+      <c r="R14" s="129"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="131">
+      <c r="T14" s="128">
         <v>131</v>
       </c>
-      <c r="U14" s="131"/>
-      <c r="V14" s="131"/>
+      <c r="U14" s="128"/>
+      <c r="V14" s="128"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10" t="str">
@@ -15218,11 +15218,11 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="63"/>
-      <c r="G15" s="136" t="s">
+      <c r="G15" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
         <v>74</v>
@@ -15231,17 +15231,17 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="128">
+      <c r="P15" s="129">
         <v>45323</v>
       </c>
-      <c r="Q15" s="128"/>
-      <c r="R15" s="128"/>
+      <c r="Q15" s="129"/>
+      <c r="R15" s="129"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="131">
+      <c r="T15" s="128">
         <v>132</v>
       </c>
-      <c r="U15" s="131"/>
-      <c r="V15" s="131"/>
+      <c r="U15" s="128"/>
+      <c r="V15" s="128"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10" t="str">
@@ -15272,11 +15272,11 @@
       <c r="C16" s="121"/>
       <c r="D16" s="121"/>
       <c r="E16" s="122"/>
-      <c r="G16" s="136" t="s">
+      <c r="G16" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="128"/>
-      <c r="I16" s="128"/>
+      <c r="H16" s="129"/>
+      <c r="I16" s="129"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
         <v>75</v>
@@ -15285,17 +15285,17 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="128">
+      <c r="P16" s="129">
         <v>45322</v>
       </c>
-      <c r="Q16" s="128"/>
-      <c r="R16" s="128"/>
+      <c r="Q16" s="129"/>
+      <c r="R16" s="129"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="131">
+      <c r="T16" s="128">
         <v>133</v>
       </c>
-      <c r="U16" s="131"/>
-      <c r="V16" s="131"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10" t="str">
@@ -15327,11 +15327,11 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="122"/>
-      <c r="G17" s="136" t="s">
+      <c r="G17" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
         <v>76</v>
@@ -15340,17 +15340,17 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="128">
+      <c r="P17" s="129">
         <v>45321</v>
       </c>
-      <c r="Q17" s="128"/>
-      <c r="R17" s="128"/>
+      <c r="Q17" s="129"/>
+      <c r="R17" s="129"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="131">
+      <c r="T17" s="128">
         <v>134</v>
       </c>
-      <c r="U17" s="131"/>
-      <c r="V17" s="131"/>
+      <c r="U17" s="128"/>
+      <c r="V17" s="128"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10" t="str">
@@ -15381,11 +15381,11 @@
       <c r="C18" s="121"/>
       <c r="D18" s="121"/>
       <c r="E18" s="122"/>
-      <c r="G18" s="136" t="s">
+      <c r="G18" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="128"/>
-      <c r="I18" s="128"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="129"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
         <v>77</v>
@@ -15394,17 +15394,17 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="128">
+      <c r="P18" s="129">
         <v>45320</v>
       </c>
-      <c r="Q18" s="128"/>
-      <c r="R18" s="128"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="129"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="131">
+      <c r="T18" s="128">
         <v>135</v>
       </c>
-      <c r="U18" s="131"/>
-      <c r="V18" s="131"/>
+      <c r="U18" s="128"/>
+      <c r="V18" s="128"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10" t="str">
@@ -15435,11 +15435,11 @@
       <c r="C19" s="121"/>
       <c r="D19" s="121"/>
       <c r="E19" s="122"/>
-      <c r="G19" s="136" t="s">
+      <c r="G19" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
         <v>78</v>
@@ -15448,17 +15448,17 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="128">
+      <c r="P19" s="129">
         <v>45319</v>
       </c>
-      <c r="Q19" s="128"/>
-      <c r="R19" s="128"/>
+      <c r="Q19" s="129"/>
+      <c r="R19" s="129"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="131">
+      <c r="T19" s="128">
         <v>136</v>
       </c>
-      <c r="U19" s="131"/>
-      <c r="V19" s="131"/>
+      <c r="U19" s="128"/>
+      <c r="V19" s="128"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10" t="str">
@@ -15489,11 +15489,11 @@
       <c r="C20" s="121"/>
       <c r="D20" s="121"/>
       <c r="E20" s="122"/>
-      <c r="G20" s="136" t="s">
+      <c r="G20" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="128"/>
-      <c r="I20" s="128"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
         <v>79</v>
@@ -15502,17 +15502,17 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="128">
+      <c r="P20" s="129">
         <v>45318</v>
       </c>
-      <c r="Q20" s="128"/>
-      <c r="R20" s="128"/>
+      <c r="Q20" s="129"/>
+      <c r="R20" s="129"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="131">
+      <c r="T20" s="128">
         <v>137</v>
       </c>
-      <c r="U20" s="131"/>
-      <c r="V20" s="131"/>
+      <c r="U20" s="128"/>
+      <c r="V20" s="128"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10" t="str">
@@ -15543,11 +15543,11 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="122"/>
-      <c r="G21" s="136" t="s">
+      <c r="G21" s="135" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="128"/>
-      <c r="I21" s="128"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10" t="s">
         <v>48</v>
@@ -15556,17 +15556,17 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="128">
+      <c r="P21" s="129">
         <v>45317</v>
       </c>
-      <c r="Q21" s="128"/>
-      <c r="R21" s="128"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="131">
+      <c r="T21" s="128">
         <v>138</v>
       </c>
-      <c r="U21" s="131"/>
-      <c r="V21" s="131"/>
+      <c r="U21" s="128"/>
+      <c r="V21" s="128"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10" t="str">
@@ -15597,11 +15597,11 @@
       <c r="C22" s="121"/>
       <c r="D22" s="121"/>
       <c r="E22" s="122"/>
-      <c r="G22" s="136" t="s">
+      <c r="G22" s="135" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="128"/>
-      <c r="I22" s="128"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
         <v>117</v>
@@ -15610,17 +15610,17 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="128">
+      <c r="P22" s="129">
         <v>45316</v>
       </c>
-      <c r="Q22" s="128"/>
-      <c r="R22" s="128"/>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="129"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="131">
+      <c r="T22" s="128">
         <v>139</v>
       </c>
-      <c r="U22" s="131"/>
-      <c r="V22" s="131"/>
+      <c r="U22" s="128"/>
+      <c r="V22" s="128"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10" t="str">
@@ -15651,11 +15651,11 @@
       <c r="C23" s="121"/>
       <c r="D23" s="121"/>
       <c r="E23" s="122"/>
-      <c r="G23" s="136" t="s">
+      <c r="G23" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
         <v>12</v>
@@ -15664,17 +15664,17 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="128">
+      <c r="P23" s="129">
         <v>45315</v>
       </c>
-      <c r="Q23" s="128"/>
-      <c r="R23" s="128"/>
+      <c r="Q23" s="129"/>
+      <c r="R23" s="129"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="131">
+      <c r="T23" s="128">
         <v>140</v>
       </c>
-      <c r="U23" s="131"/>
-      <c r="V23" s="131"/>
+      <c r="U23" s="128"/>
+      <c r="V23" s="128"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10" t="str">
@@ -15707,11 +15707,11 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="122"/>
-      <c r="G24" s="136" t="s">
+      <c r="G24" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
         <v>84</v>
@@ -15720,17 +15720,17 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="128">
+      <c r="P24" s="129">
         <v>45314</v>
       </c>
-      <c r="Q24" s="128"/>
-      <c r="R24" s="128"/>
+      <c r="Q24" s="129"/>
+      <c r="R24" s="129"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="131">
+      <c r="T24" s="128">
         <v>141</v>
       </c>
-      <c r="U24" s="131"/>
-      <c r="V24" s="131"/>
+      <c r="U24" s="128"/>
+      <c r="V24" s="128"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="str">
@@ -15761,11 +15761,11 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="122"/>
-      <c r="G25" s="136" t="s">
+      <c r="G25" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="128"/>
-      <c r="I25" s="128"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10" t="s">
         <v>69</v>
@@ -15774,17 +15774,17 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="128">
+      <c r="P25" s="129">
         <v>45313</v>
       </c>
-      <c r="Q25" s="128"/>
-      <c r="R25" s="128"/>
+      <c r="Q25" s="129"/>
+      <c r="R25" s="129"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="131">
+      <c r="T25" s="128">
         <v>142</v>
       </c>
-      <c r="U25" s="131"/>
-      <c r="V25" s="131"/>
+      <c r="U25" s="128"/>
+      <c r="V25" s="128"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10" t="str">
@@ -15815,11 +15815,11 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="122"/>
-      <c r="G26" s="136" t="s">
+      <c r="G26" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="128"/>
-      <c r="I26" s="128"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="s">
         <v>70</v>
@@ -15828,17 +15828,17 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="128">
+      <c r="P26" s="129">
         <v>45312</v>
       </c>
-      <c r="Q26" s="128"/>
-      <c r="R26" s="128"/>
+      <c r="Q26" s="129"/>
+      <c r="R26" s="129"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="131">
+      <c r="T26" s="128">
         <v>143</v>
       </c>
-      <c r="U26" s="131"/>
-      <c r="V26" s="131"/>
+      <c r="U26" s="128"/>
+      <c r="V26" s="128"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10" t="str">
@@ -15869,11 +15869,11 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="122"/>
-      <c r="G27" s="136" t="s">
+      <c r="G27" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10" t="s">
         <v>71</v>
@@ -15882,17 +15882,17 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="128">
+      <c r="P27" s="129">
         <v>45311</v>
       </c>
-      <c r="Q27" s="128"/>
-      <c r="R27" s="128"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="129"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="131">
+      <c r="T27" s="128">
         <v>144</v>
       </c>
-      <c r="U27" s="131"/>
-      <c r="V27" s="131"/>
+      <c r="U27" s="128"/>
+      <c r="V27" s="128"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10" t="str">
@@ -15923,11 +15923,11 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="122"/>
-      <c r="G28" s="136" t="s">
+      <c r="G28" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="128"/>
-      <c r="I28" s="128"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10" t="s">
         <v>72</v>
@@ -15936,17 +15936,17 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="128">
+      <c r="P28" s="129">
         <v>45310</v>
       </c>
-      <c r="Q28" s="128"/>
-      <c r="R28" s="128"/>
+      <c r="Q28" s="129"/>
+      <c r="R28" s="129"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="131">
+      <c r="T28" s="128">
         <v>145</v>
       </c>
-      <c r="U28" s="131"/>
-      <c r="V28" s="131"/>
+      <c r="U28" s="128"/>
+      <c r="V28" s="128"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10" t="str">
@@ -15977,11 +15977,11 @@
       <c r="C29" s="121"/>
       <c r="D29" s="121"/>
       <c r="E29" s="122"/>
-      <c r="G29" s="136" t="s">
+      <c r="G29" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10" t="s">
         <v>73</v>
@@ -15990,17 +15990,17 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="128">
+      <c r="P29" s="129">
         <v>45309</v>
       </c>
-      <c r="Q29" s="128"/>
-      <c r="R29" s="128"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="131">
+      <c r="T29" s="128">
         <v>146</v>
       </c>
-      <c r="U29" s="131"/>
-      <c r="V29" s="131"/>
+      <c r="U29" s="128"/>
+      <c r="V29" s="128"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10" t="str">
@@ -16031,11 +16031,11 @@
       <c r="C30" s="121"/>
       <c r="D30" s="121"/>
       <c r="E30" s="122"/>
-      <c r="G30" s="135" t="s">
+      <c r="G30" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="129"/>
-      <c r="I30" s="129"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>74</v>
@@ -16044,17 +16044,17 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="129">
+      <c r="P30" s="131">
         <v>45308</v>
       </c>
-      <c r="Q30" s="129"/>
-      <c r="R30" s="129"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
       <c r="S30" s="2"/>
-      <c r="T30" s="132">
+      <c r="T30" s="130">
         <v>147</v>
       </c>
-      <c r="U30" s="132"/>
-      <c r="V30" s="132"/>
+      <c r="U30" s="130"/>
+      <c r="V30" s="130"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2" t="str">
@@ -16082,27 +16082,64 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="T30:V30"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
@@ -16119,64 +16156,27 @@
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="T30:V30"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="T17:V17"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="T19:V19"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="T23:V23"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="T25:V25"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected the bar charts in the dashboard for transactions.
</commit_message>
<xml_diff>
--- a/docs/Mockups.xlsx
+++ b/docs/Mockups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="14" r:id="rId1"/>
@@ -1514,14 +1514,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1529,13 +1529,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1544,20 +1538,29 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1566,9 +1569,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1584,6 +1584,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1604,15 +1616,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1621,9 +1624,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1685,13 +1685,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>210764</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19850</xdr:rowOff>
+      <xdr:colOff>125027</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>181745</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1705,7 +1705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1771650" y="1323975"/>
-          <a:ext cx="8697539" cy="5734850"/>
+          <a:ext cx="8611802" cy="5515745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3143,12 +3143,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -3503,6 +3503,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="B30:E30"/>
@@ -3519,18 +3531,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3628,12 +3628,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -3716,11 +3716,11 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="129">
+      <c r="L8" s="128">
         <v>45336</v>
       </c>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
+      <c r="M8" s="128"/>
+      <c r="N8" s="128"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
         <v>127</v>
@@ -3770,11 +3770,11 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="129">
+      <c r="L9" s="128">
         <v>45324</v>
       </c>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
         <v>128</v>
@@ -3826,11 +3826,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="129">
+      <c r="L10" s="128">
         <v>45241</v>
       </c>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
       <c r="O10" s="10"/>
       <c r="P10" s="9" t="s">
         <v>127</v>
@@ -3880,11 +3880,11 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="129">
+      <c r="L11" s="128">
         <v>45281</v>
       </c>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
         <v>129</v>
@@ -3934,11 +3934,11 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="129">
+      <c r="L12" s="128">
         <v>45220</v>
       </c>
-      <c r="M12" s="129"/>
-      <c r="N12" s="129"/>
+      <c r="M12" s="128"/>
+      <c r="N12" s="128"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
         <v>130</v>
@@ -4737,6 +4737,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -4753,21 +4768,6 @@
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4882,12 +4882,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -5462,6 +5462,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B24:E24"/>
@@ -5478,17 +5489,6 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5586,25 +5586,25 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="N5" s="138" t="s">
+      <c r="N5" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="O5" s="139"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="140"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="141"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121" t="s">
@@ -5680,17 +5680,17 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="129">
+      <c r="K8" s="128">
         <v>45353</v>
       </c>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="128">
+      <c r="O8" s="131">
         <v>10</v>
       </c>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="128"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10" t="s">
         <v>127</v>
@@ -5706,9 +5706,9 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
       <c r="AB8" s="10"/>
-      <c r="AC8" s="141"/>
-      <c r="AD8" s="141"/>
-      <c r="AE8" s="141"/>
+      <c r="AC8" s="138"/>
+      <c r="AD8" s="138"/>
+      <c r="AE8" s="138"/>
       <c r="AF8" s="86"/>
       <c r="AG8" s="10" t="s">
         <v>175</v>
@@ -5736,17 +5736,17 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="129">
+      <c r="K9" s="128">
         <v>45353</v>
       </c>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="128">
+      <c r="O9" s="131">
         <v>10</v>
       </c>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="128"/>
+      <c r="P9" s="131"/>
+      <c r="Q9" s="131"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10" t="s">
         <v>127</v>
@@ -5762,9 +5762,9 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
-      <c r="AC9" s="141"/>
-      <c r="AD9" s="141"/>
-      <c r="AE9" s="141"/>
+      <c r="AC9" s="138"/>
+      <c r="AD9" s="138"/>
+      <c r="AE9" s="138"/>
       <c r="AF9" s="86"/>
       <c r="AG9" s="10" t="s">
         <v>175</v>
@@ -5788,13 +5788,13 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="128"/>
-      <c r="Q10" s="128"/>
+      <c r="O10" s="131"/>
+      <c r="P10" s="131"/>
+      <c r="Q10" s="131"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5806,9 +5806,9 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
-      <c r="AC10" s="141"/>
-      <c r="AD10" s="141"/>
-      <c r="AE10" s="141"/>
+      <c r="AC10" s="138"/>
+      <c r="AD10" s="138"/>
+      <c r="AE10" s="138"/>
       <c r="AF10" s="86"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="86"/>
@@ -5834,17 +5834,17 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="129">
+      <c r="K11" s="128">
         <v>45354</v>
       </c>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="128">
+      <c r="O11" s="131">
         <v>5</v>
       </c>
-      <c r="P11" s="128"/>
-      <c r="Q11" s="128"/>
+      <c r="P11" s="131"/>
+      <c r="Q11" s="131"/>
       <c r="R11" s="10"/>
       <c r="S11" s="9" t="s">
         <v>130</v>
@@ -5860,9 +5860,9 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
-      <c r="AC11" s="141"/>
-      <c r="AD11" s="141"/>
-      <c r="AE11" s="141"/>
+      <c r="AC11" s="138"/>
+      <c r="AD11" s="138"/>
+      <c r="AE11" s="138"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="9" t="s">
         <v>176</v>
@@ -5888,17 +5888,17 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="129">
+      <c r="K12" s="128">
         <v>45355</v>
       </c>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="128">
+      <c r="O12" s="131">
         <v>10</v>
       </c>
-      <c r="P12" s="128"/>
-      <c r="Q12" s="128"/>
+      <c r="P12" s="131"/>
+      <c r="Q12" s="131"/>
       <c r="R12" s="10"/>
       <c r="S12" s="9" t="s">
         <v>128</v>
@@ -5944,17 +5944,17 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="129">
+      <c r="K13" s="128">
         <v>45356</v>
       </c>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="128">
+      <c r="O13" s="131">
         <v>20</v>
       </c>
-      <c r="P13" s="128"/>
-      <c r="Q13" s="128"/>
+      <c r="P13" s="131"/>
+      <c r="Q13" s="131"/>
       <c r="R13" s="10"/>
       <c r="S13" s="9" t="s">
         <v>129</v>
@@ -6187,26 +6187,26 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="128">
+      <c r="M21" s="131">
         <v>30</v>
       </c>
-      <c r="N21" s="128"/>
-      <c r="O21" s="128"/>
+      <c r="N21" s="131"/>
+      <c r="O21" s="131"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="128">
+      <c r="Q21" s="131">
         <v>35</v>
       </c>
-      <c r="R21" s="128"/>
-      <c r="S21" s="128"/>
-      <c r="T21" s="128"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="128">
+      <c r="V21" s="131">
         <f>M21-Q21</f>
         <v>-5</v>
       </c>
-      <c r="W21" s="128"/>
-      <c r="X21" s="128"/>
-      <c r="Y21" s="128"/>
+      <c r="W21" s="131"/>
+      <c r="X21" s="131"/>
+      <c r="Y21" s="131"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="44"/>
     </row>
@@ -6223,26 +6223,26 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="128">
+      <c r="M22" s="131">
         <v>20</v>
       </c>
-      <c r="N22" s="128"/>
-      <c r="O22" s="128"/>
+      <c r="N22" s="131"/>
+      <c r="O22" s="131"/>
       <c r="P22" s="10"/>
-      <c r="Q22" s="128">
+      <c r="Q22" s="131">
         <v>10</v>
       </c>
-      <c r="R22" s="128"/>
-      <c r="S22" s="128"/>
-      <c r="T22" s="128"/>
+      <c r="R22" s="131"/>
+      <c r="S22" s="131"/>
+      <c r="T22" s="131"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="128">
+      <c r="V22" s="131">
         <f>M22-Q22</f>
         <v>10</v>
       </c>
-      <c r="W22" s="128"/>
-      <c r="X22" s="128"/>
-      <c r="Y22" s="128"/>
+      <c r="W22" s="131"/>
+      <c r="X22" s="131"/>
+      <c r="Y22" s="131"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="44"/>
     </row>
@@ -6259,26 +6259,26 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="128">
+      <c r="M23" s="131">
         <v>5</v>
       </c>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
+      <c r="N23" s="131"/>
+      <c r="O23" s="131"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="128">
+      <c r="Q23" s="131">
         <v>10</v>
       </c>
-      <c r="R23" s="128"/>
-      <c r="S23" s="128"/>
-      <c r="T23" s="128"/>
+      <c r="R23" s="131"/>
+      <c r="S23" s="131"/>
+      <c r="T23" s="131"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="128">
+      <c r="V23" s="131">
         <f>M23-Q23</f>
         <v>-5</v>
       </c>
-      <c r="W23" s="128"/>
-      <c r="X23" s="128"/>
-      <c r="Y23" s="128"/>
+      <c r="W23" s="131"/>
+      <c r="X23" s="131"/>
+      <c r="Y23" s="131"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="44"/>
     </row>
@@ -6295,26 +6295,26 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="128">
+      <c r="M24" s="131">
         <v>10</v>
       </c>
-      <c r="N24" s="128"/>
-      <c r="O24" s="128"/>
+      <c r="N24" s="131"/>
+      <c r="O24" s="131"/>
       <c r="P24" s="10"/>
-      <c r="Q24" s="128">
+      <c r="Q24" s="131">
         <v>10</v>
       </c>
-      <c r="R24" s="128"/>
-      <c r="S24" s="128"/>
-      <c r="T24" s="128"/>
+      <c r="R24" s="131"/>
+      <c r="S24" s="131"/>
+      <c r="T24" s="131"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="128">
+      <c r="V24" s="131">
         <f>M24-Q24</f>
         <v>0</v>
       </c>
-      <c r="W24" s="128"/>
-      <c r="X24" s="128"/>
-      <c r="Y24" s="128"/>
+      <c r="W24" s="131"/>
+      <c r="X24" s="131"/>
+      <c r="Y24" s="131"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="44"/>
     </row>
@@ -6380,36 +6380,15 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="AC11:AE11"/>
-    <mergeCell ref="AC9:AE9"/>
-    <mergeCell ref="AC10:AE10"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V23:Y23"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="Q22:T22"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q24:T24"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="M21:O21"/>
@@ -6426,15 +6405,36 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="Q21:T21"/>
-    <mergeCell ref="Q22:T22"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="AC11:AE11"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="AC10:AE10"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="O11:Q11"/>
   </mergeCells>
   <conditionalFormatting sqref="V21:Y24">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -6559,12 +6559,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -7083,6 +7083,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="H8:R8"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -7099,20 +7113,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7517,10 +7517,10 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="44"/>
-      <c r="J46" s="138" t="s">
+      <c r="J46" s="139" t="s">
         <v>54</v>
       </c>
-      <c r="K46" s="140"/>
+      <c r="K46" s="141"/>
       <c r="M46" s="144"/>
       <c r="N46" s="144"/>
       <c r="O46" s="144"/>
@@ -7939,46 +7939,46 @@
       <c r="C5" s="121"/>
       <c r="D5" s="121"/>
       <c r="E5" s="146"/>
-      <c r="G5" s="159" t="s">
+      <c r="G5" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="159"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
-      <c r="AD5" s="159"/>
-      <c r="AE5" s="159"/>
-      <c r="AF5" s="159"/>
-      <c r="AG5" s="159"/>
-      <c r="AH5" s="159"/>
-      <c r="AI5" s="159"/>
-      <c r="AJ5" s="159"/>
-      <c r="AK5" s="159"/>
-      <c r="AL5" s="159"/>
-      <c r="AM5" s="159"/>
-      <c r="AN5" s="159"/>
-      <c r="AO5" s="159"/>
-      <c r="AP5" s="159"/>
-      <c r="AQ5" s="159"/>
-      <c r="AR5" s="159"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147"/>
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="147"/>
+      <c r="AI5" s="147"/>
+      <c r="AJ5" s="147"/>
+      <c r="AK5" s="147"/>
+      <c r="AL5" s="147"/>
+      <c r="AM5" s="147"/>
+      <c r="AN5" s="147"/>
+      <c r="AO5" s="147"/>
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -8095,13 +8095,13 @@
       <c r="C8" s="121"/>
       <c r="D8" s="121"/>
       <c r="E8" s="146"/>
-      <c r="G8" s="156" t="s">
+      <c r="G8" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="157"/>
-      <c r="K8" s="158"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="159"/>
       <c r="L8" s="25" t="s">
         <v>25</v>
       </c>
@@ -8210,13 +8210,13 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="146"/>
-      <c r="G9" s="153" t="s">
+      <c r="G9" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="155"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="150"/>
       <c r="L9" s="24">
         <f t="shared" ref="L9:M12" si="0">SUM(M9:AQ9)</f>
         <v>610</v>
@@ -8324,13 +8324,13 @@
       <c r="C10" s="121"/>
       <c r="D10" s="121"/>
       <c r="E10" s="146"/>
-      <c r="G10" s="153" t="s">
+      <c r="G10" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="155"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="150"/>
       <c r="L10" s="24">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -8380,13 +8380,13 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="146"/>
-      <c r="G11" s="153" t="s">
+      <c r="G11" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="155"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
+      <c r="K11" s="150"/>
       <c r="L11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8432,13 +8432,13 @@
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
       <c r="E12" s="146"/>
-      <c r="G12" s="153" t="s">
+      <c r="G12" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="155"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="150"/>
       <c r="L12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8484,13 +8484,13 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="146"/>
-      <c r="G13" s="153" t="s">
+      <c r="G13" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="155"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="150"/>
       <c r="L13" s="24">
         <v>500</v>
       </c>
@@ -8541,13 +8541,13 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="146"/>
-      <c r="G14" s="153" t="s">
+      <c r="G14" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="155"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="150"/>
       <c r="L14" s="24">
         <f>SUM(M14:AQ14)</f>
         <v>246</v>
@@ -8595,13 +8595,13 @@
       <c r="C15" s="121"/>
       <c r="D15" s="121"/>
       <c r="E15" s="146"/>
-      <c r="G15" s="153" t="s">
+      <c r="G15" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="155"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="149"/>
+      <c r="K15" s="150"/>
       <c r="L15" s="24">
         <f>SUM(M15:AQ15)</f>
         <v>220</v>
@@ -8649,13 +8649,13 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="G16" s="147" t="s">
+      <c r="G16" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="149"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="153"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="11"/>
@@ -8695,13 +8695,13 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="146"/>
-      <c r="G17" s="150" t="s">
+      <c r="G17" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="152"/>
+      <c r="H17" s="155"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="155"/>
+      <c r="K17" s="156"/>
       <c r="L17" s="26">
         <f>SUM(L9:L16)</f>
         <v>1976</v>
@@ -8863,46 +8863,46 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="146"/>
-      <c r="G21" s="159" t="s">
+      <c r="G21" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="159"/>
-      <c r="O21" s="159"/>
-      <c r="P21" s="159"/>
-      <c r="Q21" s="159"/>
-      <c r="R21" s="159"/>
-      <c r="S21" s="159"/>
-      <c r="T21" s="159"/>
-      <c r="U21" s="159"/>
-      <c r="V21" s="159"/>
-      <c r="W21" s="159"/>
-      <c r="X21" s="159"/>
-      <c r="Y21" s="159"/>
-      <c r="Z21" s="159"/>
-      <c r="AA21" s="159"/>
-      <c r="AB21" s="159"/>
-      <c r="AC21" s="159"/>
-      <c r="AD21" s="159"/>
-      <c r="AE21" s="159"/>
-      <c r="AF21" s="159"/>
-      <c r="AG21" s="159"/>
-      <c r="AH21" s="159"/>
-      <c r="AI21" s="159"/>
-      <c r="AJ21" s="159"/>
-      <c r="AK21" s="159"/>
-      <c r="AL21" s="159"/>
-      <c r="AM21" s="159"/>
-      <c r="AN21" s="159"/>
-      <c r="AO21" s="159"/>
-      <c r="AP21" s="159"/>
-      <c r="AQ21" s="159"/>
-      <c r="AR21" s="159"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="147"/>
+      <c r="K21" s="147"/>
+      <c r="L21" s="147"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="147"/>
+      <c r="O21" s="147"/>
+      <c r="P21" s="147"/>
+      <c r="Q21" s="147"/>
+      <c r="R21" s="147"/>
+      <c r="S21" s="147"/>
+      <c r="T21" s="147"/>
+      <c r="U21" s="147"/>
+      <c r="V21" s="147"/>
+      <c r="W21" s="147"/>
+      <c r="X21" s="147"/>
+      <c r="Y21" s="147"/>
+      <c r="Z21" s="147"/>
+      <c r="AA21" s="147"/>
+      <c r="AB21" s="147"/>
+      <c r="AC21" s="147"/>
+      <c r="AD21" s="147"/>
+      <c r="AE21" s="147"/>
+      <c r="AF21" s="147"/>
+      <c r="AG21" s="147"/>
+      <c r="AH21" s="147"/>
+      <c r="AI21" s="147"/>
+      <c r="AJ21" s="147"/>
+      <c r="AK21" s="147"/>
+      <c r="AL21" s="147"/>
+      <c r="AM21" s="147"/>
+      <c r="AN21" s="147"/>
+      <c r="AO21" s="147"/>
+      <c r="AP21" s="147"/>
+      <c r="AQ21" s="147"/>
+      <c r="AR21" s="147"/>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B22" s="121"/>
@@ -9015,13 +9015,13 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="146"/>
-      <c r="G24" s="156" t="s">
+      <c r="G24" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="158"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="158"/>
+      <c r="K24" s="159"/>
       <c r="L24" s="25" t="s">
         <v>25</v>
       </c>
@@ -9127,13 +9127,13 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="146"/>
-      <c r="G25" s="153" t="s">
+      <c r="G25" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="154"/>
-      <c r="I25" s="154"/>
-      <c r="J25" s="154"/>
-      <c r="K25" s="155"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="150"/>
       <c r="L25" s="24">
         <f>SUM(M25:AQ25)</f>
         <v>610</v>
@@ -9241,13 +9241,13 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="146"/>
-      <c r="G26" s="153" t="s">
+      <c r="G26" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="154"/>
-      <c r="I26" s="154"/>
-      <c r="J26" s="154"/>
-      <c r="K26" s="155"/>
+      <c r="H26" s="149"/>
+      <c r="I26" s="149"/>
+      <c r="J26" s="149"/>
+      <c r="K26" s="150"/>
       <c r="L26" s="24">
         <f>SUM(M26:AQ26)</f>
         <v>400</v>
@@ -9297,13 +9297,13 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="146"/>
-      <c r="G27" s="147" t="s">
+      <c r="G27" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="149"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="152"/>
+      <c r="K27" s="153"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="11"/>
@@ -9343,13 +9343,13 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="146"/>
-      <c r="G28" s="150" t="s">
+      <c r="G28" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="151"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="151"/>
-      <c r="K28" s="152"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="26">
         <f>SUM(L25:L27)</f>
         <v>1010</v>
@@ -9507,15 +9507,24 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G21:AR21"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="G5:AR5"/>
     <mergeCell ref="G9:K9"/>
@@ -9532,24 +9541,15 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G21:AR21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:L16">
     <cfRule type="dataBar" priority="2">
@@ -9708,43 +9708,43 @@
       <c r="G5" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="159"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
-      <c r="AD5" s="159"/>
-      <c r="AE5" s="159"/>
-      <c r="AF5" s="159"/>
-      <c r="AG5" s="159"/>
-      <c r="AH5" s="159"/>
-      <c r="AI5" s="159"/>
-      <c r="AJ5" s="159"/>
-      <c r="AK5" s="159"/>
-      <c r="AL5" s="159"/>
-      <c r="AM5" s="159"/>
-      <c r="AN5" s="159"/>
-      <c r="AO5" s="159"/>
-      <c r="AP5" s="159"/>
-      <c r="AQ5" s="159"/>
-      <c r="AR5" s="159"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147"/>
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="147"/>
+      <c r="AI5" s="147"/>
+      <c r="AJ5" s="147"/>
+      <c r="AK5" s="147"/>
+      <c r="AL5" s="147"/>
+      <c r="AM5" s="147"/>
+      <c r="AN5" s="147"/>
+      <c r="AO5" s="147"/>
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -9753,11 +9753,11 @@
       <c r="E6" s="146"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="161"/>
       <c r="G7" s="40" t="s">
         <v>28</v>
@@ -10216,23 +10216,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:AR5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:AR5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11216,8 +11216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AU20" sqref="AU20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="BB27" sqref="BB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11306,24 +11306,24 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="G5" s="120" t="s">
         <v>168</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="125" t="s">
+      <c r="K5" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
@@ -11500,6 +11500,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B31:E31"/>
@@ -11516,20 +11530,6 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:N5">
@@ -11545,7 +11545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
@@ -11643,12 +11643,12 @@
       <c r="E5" s="122"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -11798,14 +11798,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -11818,12 +11816,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11922,12 +11922,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -12846,14 +12846,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -12866,12 +12864,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12983,12 +12983,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -13229,14 +13229,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -13249,12 +13247,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13352,12 +13352,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -13387,11 +13387,11 @@
       <c r="K7" s="68"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="132" t="s">
+      <c r="N7" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="132"/>
-      <c r="P7" s="132"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
       <c r="Q7" s="68"/>
       <c r="R7" s="68" t="s">
         <v>25</v>
@@ -13428,17 +13428,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="129">
+      <c r="N8" s="128">
         <v>45334</v>
       </c>
-      <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
+      <c r="O8" s="128"/>
+      <c r="P8" s="128"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="128">
+      <c r="R8" s="131">
         <v>500</v>
       </c>
-      <c r="S8" s="128"/>
-      <c r="T8" s="128"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="131"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -13460,17 +13460,17 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="129">
+      <c r="N9" s="128">
         <v>45334</v>
       </c>
-      <c r="O9" s="129"/>
-      <c r="P9" s="129"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="128"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="128">
+      <c r="R9" s="131">
         <v>501</v>
       </c>
-      <c r="S9" s="128"/>
-      <c r="T9" s="128"/>
+      <c r="S9" s="131"/>
+      <c r="T9" s="131"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -13492,17 +13492,17 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="129">
+      <c r="N10" s="128">
         <v>45334</v>
       </c>
-      <c r="O10" s="129"/>
-      <c r="P10" s="129"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="128"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="128">
+      <c r="R10" s="131">
         <v>502</v>
       </c>
-      <c r="S10" s="128"/>
-      <c r="T10" s="128"/>
+      <c r="S10" s="131"/>
+      <c r="T10" s="131"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -13524,17 +13524,17 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="129">
+      <c r="N11" s="128">
         <v>45334</v>
       </c>
-      <c r="O11" s="129"/>
-      <c r="P11" s="129"/>
+      <c r="O11" s="128"/>
+      <c r="P11" s="128"/>
       <c r="Q11" s="10"/>
-      <c r="R11" s="128">
+      <c r="R11" s="131">
         <v>503</v>
       </c>
-      <c r="S11" s="128"/>
-      <c r="T11" s="128"/>
+      <c r="S11" s="131"/>
+      <c r="T11" s="131"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -13556,17 +13556,17 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="129">
+      <c r="N12" s="128">
         <v>45334</v>
       </c>
-      <c r="O12" s="129"/>
-      <c r="P12" s="129"/>
+      <c r="O12" s="128"/>
+      <c r="P12" s="128"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="128">
+      <c r="R12" s="131">
         <v>504</v>
       </c>
-      <c r="S12" s="128"/>
-      <c r="T12" s="128"/>
+      <c r="S12" s="131"/>
+      <c r="T12" s="131"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -13588,17 +13588,17 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="129">
+      <c r="N13" s="128">
         <v>45334</v>
       </c>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
+      <c r="O13" s="128"/>
+      <c r="P13" s="128"/>
       <c r="Q13" s="10"/>
-      <c r="R13" s="128">
+      <c r="R13" s="131">
         <v>505</v>
       </c>
-      <c r="S13" s="128"/>
-      <c r="T13" s="128"/>
+      <c r="S13" s="131"/>
+      <c r="T13" s="131"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -13620,17 +13620,17 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="129">
+      <c r="N14" s="128">
         <v>45334</v>
       </c>
-      <c r="O14" s="129"/>
-      <c r="P14" s="129"/>
+      <c r="O14" s="128"/>
+      <c r="P14" s="128"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="128">
+      <c r="R14" s="131">
         <v>506</v>
       </c>
-      <c r="S14" s="128"/>
-      <c r="T14" s="128"/>
+      <c r="S14" s="131"/>
+      <c r="T14" s="131"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -13652,17 +13652,17 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="129">
+      <c r="N15" s="128">
         <v>45334</v>
       </c>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="128">
+      <c r="R15" s="131">
         <v>507</v>
       </c>
-      <c r="S15" s="128"/>
-      <c r="T15" s="128"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
@@ -13684,17 +13684,17 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="129">
+      <c r="N16" s="128">
         <v>45334</v>
       </c>
-      <c r="O16" s="129"/>
-      <c r="P16" s="129"/>
+      <c r="O16" s="128"/>
+      <c r="P16" s="128"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="128">
+      <c r="R16" s="131">
         <v>508</v>
       </c>
-      <c r="S16" s="128"/>
-      <c r="T16" s="128"/>
+      <c r="S16" s="131"/>
+      <c r="T16" s="131"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -13717,17 +13717,17 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="129">
+      <c r="N17" s="128">
         <v>45334</v>
       </c>
-      <c r="O17" s="129"/>
-      <c r="P17" s="129"/>
+      <c r="O17" s="128"/>
+      <c r="P17" s="128"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="128">
+      <c r="R17" s="131">
         <v>509</v>
       </c>
-      <c r="S17" s="128"/>
-      <c r="T17" s="128"/>
+      <c r="S17" s="131"/>
+      <c r="T17" s="131"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -13749,17 +13749,17 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="129">
+      <c r="N18" s="128">
         <v>45334</v>
       </c>
-      <c r="O18" s="129"/>
-      <c r="P18" s="129"/>
+      <c r="O18" s="128"/>
+      <c r="P18" s="128"/>
       <c r="Q18" s="10"/>
-      <c r="R18" s="128">
+      <c r="R18" s="131">
         <v>510</v>
       </c>
-      <c r="S18" s="128"/>
-      <c r="T18" s="128"/>
+      <c r="S18" s="131"/>
+      <c r="T18" s="131"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
@@ -13781,17 +13781,17 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="129">
+      <c r="N19" s="128">
         <v>45334</v>
       </c>
-      <c r="O19" s="129"/>
-      <c r="P19" s="129"/>
+      <c r="O19" s="128"/>
+      <c r="P19" s="128"/>
       <c r="Q19" s="10"/>
-      <c r="R19" s="128">
+      <c r="R19" s="131">
         <v>511</v>
       </c>
-      <c r="S19" s="128"/>
-      <c r="T19" s="128"/>
+      <c r="S19" s="131"/>
+      <c r="T19" s="131"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -13813,17 +13813,17 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="129">
+      <c r="N20" s="128">
         <v>45334</v>
       </c>
-      <c r="O20" s="129"/>
-      <c r="P20" s="129"/>
+      <c r="O20" s="128"/>
+      <c r="P20" s="128"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="128">
+      <c r="R20" s="131">
         <v>512</v>
       </c>
-      <c r="S20" s="128"/>
-      <c r="T20" s="128"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
@@ -13845,17 +13845,17 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="129">
+      <c r="N21" s="128">
         <v>45292</v>
       </c>
-      <c r="O21" s="129"/>
-      <c r="P21" s="129"/>
+      <c r="O21" s="128"/>
+      <c r="P21" s="128"/>
       <c r="Q21" s="10"/>
-      <c r="R21" s="128">
+      <c r="R21" s="131">
         <v>513</v>
       </c>
-      <c r="S21" s="128"/>
-      <c r="T21" s="128"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -13877,17 +13877,17 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="129">
+      <c r="N22" s="128">
         <v>45292</v>
       </c>
-      <c r="O22" s="129"/>
-      <c r="P22" s="129"/>
+      <c r="O22" s="128"/>
+      <c r="P22" s="128"/>
       <c r="Q22" s="10"/>
-      <c r="R22" s="128">
+      <c r="R22" s="131">
         <v>514</v>
       </c>
-      <c r="S22" s="128"/>
-      <c r="T22" s="128"/>
+      <c r="S22" s="131"/>
+      <c r="T22" s="131"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
@@ -13909,17 +13909,17 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="129">
+      <c r="N23" s="128">
         <v>45292</v>
       </c>
-      <c r="O23" s="129"/>
-      <c r="P23" s="129"/>
+      <c r="O23" s="128"/>
+      <c r="P23" s="128"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="128">
+      <c r="R23" s="131">
         <v>515</v>
       </c>
-      <c r="S23" s="128"/>
-      <c r="T23" s="128"/>
+      <c r="S23" s="131"/>
+      <c r="T23" s="131"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -13941,17 +13941,17 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="129">
+      <c r="N24" s="128">
         <v>45292</v>
       </c>
-      <c r="O24" s="129"/>
-      <c r="P24" s="129"/>
+      <c r="O24" s="128"/>
+      <c r="P24" s="128"/>
       <c r="Q24" s="10"/>
-      <c r="R24" s="128">
+      <c r="R24" s="131">
         <v>516</v>
       </c>
-      <c r="S24" s="128"/>
-      <c r="T24" s="128"/>
+      <c r="S24" s="131"/>
+      <c r="T24" s="131"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -13973,17 +13973,17 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="129">
+      <c r="N25" s="128">
         <v>45292</v>
       </c>
-      <c r="O25" s="129"/>
-      <c r="P25" s="129"/>
+      <c r="O25" s="128"/>
+      <c r="P25" s="128"/>
       <c r="Q25" s="10"/>
-      <c r="R25" s="128">
+      <c r="R25" s="131">
         <v>517</v>
       </c>
-      <c r="S25" s="128"/>
-      <c r="T25" s="128"/>
+      <c r="S25" s="131"/>
+      <c r="T25" s="131"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -14005,17 +14005,17 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="129">
+      <c r="N26" s="128">
         <v>45292</v>
       </c>
-      <c r="O26" s="129"/>
-      <c r="P26" s="129"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="128"/>
       <c r="Q26" s="10"/>
-      <c r="R26" s="128">
+      <c r="R26" s="131">
         <v>518</v>
       </c>
-      <c r="S26" s="128"/>
-      <c r="T26" s="128"/>
+      <c r="S26" s="131"/>
+      <c r="T26" s="131"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -14037,17 +14037,17 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="129">
+      <c r="N27" s="128">
         <v>45292</v>
       </c>
-      <c r="O27" s="129"/>
-      <c r="P27" s="129"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="128"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="128">
+      <c r="R27" s="131">
         <v>519</v>
       </c>
-      <c r="S27" s="128"/>
-      <c r="T27" s="128"/>
+      <c r="S27" s="131"/>
+      <c r="T27" s="131"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
@@ -14069,17 +14069,17 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="129">
+      <c r="N28" s="128">
         <v>45292</v>
       </c>
-      <c r="O28" s="129"/>
-      <c r="P28" s="129"/>
+      <c r="O28" s="128"/>
+      <c r="P28" s="128"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="128">
+      <c r="R28" s="131">
         <v>520</v>
       </c>
-      <c r="S28" s="128"/>
-      <c r="T28" s="128"/>
+      <c r="S28" s="131"/>
+      <c r="T28" s="131"/>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
@@ -14101,17 +14101,17 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="129">
+      <c r="N29" s="128">
         <v>45292</v>
       </c>
-      <c r="O29" s="129"/>
-      <c r="P29" s="129"/>
+      <c r="O29" s="128"/>
+      <c r="P29" s="128"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="128">
+      <c r="R29" s="131">
         <v>521</v>
       </c>
-      <c r="S29" s="128"/>
-      <c r="T29" s="128"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="131"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
@@ -14133,17 +14133,17 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="131">
+      <c r="N30" s="129">
         <v>45292</v>
       </c>
-      <c r="O30" s="131"/>
-      <c r="P30" s="131"/>
+      <c r="O30" s="129"/>
+      <c r="P30" s="129"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="130">
+      <c r="R30" s="132">
         <v>522</v>
       </c>
-      <c r="S30" s="130"/>
-      <c r="T30" s="130"/>
+      <c r="S30" s="132"/>
+      <c r="T30" s="132"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -14153,6 +14153,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="R26:T26"/>
     <mergeCell ref="N27:P27"/>
     <mergeCell ref="N28:P28"/>
     <mergeCell ref="N29:P29"/>
@@ -14169,63 +14226,6 @@
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14337,12 +14337,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -14631,6 +14631,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H12:J12"/>
@@ -14647,18 +14659,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14758,12 +14758,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -14838,11 +14838,11 @@
       <c r="C8" s="126"/>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
-      <c r="G8" s="135" t="s">
+      <c r="G8" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10" t="s">
         <v>12</v>
@@ -14851,17 +14851,17 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="129">
+      <c r="P8" s="128">
         <v>45330</v>
       </c>
-      <c r="Q8" s="129"/>
-      <c r="R8" s="129"/>
+      <c r="Q8" s="128"/>
+      <c r="R8" s="128"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="128">
+      <c r="T8" s="131">
         <v>125</v>
       </c>
-      <c r="U8" s="128"/>
-      <c r="V8" s="128"/>
+      <c r="U8" s="131"/>
+      <c r="V8" s="131"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10" t="str">
@@ -14892,11 +14892,11 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="122"/>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>84</v>
@@ -14905,17 +14905,17 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="129">
+      <c r="P9" s="128">
         <v>45329</v>
       </c>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
+      <c r="Q9" s="128"/>
+      <c r="R9" s="128"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="128">
+      <c r="T9" s="131">
         <v>120</v>
       </c>
-      <c r="U9" s="128"/>
-      <c r="V9" s="128"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="131"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10" t="str">
@@ -14948,11 +14948,11 @@
       <c r="C10" s="126"/>
       <c r="D10" s="126"/>
       <c r="E10" s="127"/>
-      <c r="G10" s="135" t="s">
+      <c r="G10" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="129"/>
-      <c r="I10" s="129"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
         <v>69</v>
@@ -14961,17 +14961,17 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="129">
+      <c r="P10" s="128">
         <v>45328</v>
       </c>
-      <c r="Q10" s="129"/>
-      <c r="R10" s="129"/>
+      <c r="Q10" s="128"/>
+      <c r="R10" s="128"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="128">
+      <c r="T10" s="131">
         <v>127</v>
       </c>
-      <c r="U10" s="128"/>
-      <c r="V10" s="128"/>
+      <c r="U10" s="131"/>
+      <c r="V10" s="131"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10" t="str">
@@ -15002,11 +15002,11 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="122"/>
-      <c r="G11" s="135" t="s">
+      <c r="G11" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
         <v>70</v>
@@ -15015,17 +15015,17 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="129">
+      <c r="P11" s="128">
         <v>45327</v>
       </c>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
+      <c r="Q11" s="128"/>
+      <c r="R11" s="128"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="128">
+      <c r="T11" s="131">
         <v>128</v>
       </c>
-      <c r="U11" s="128"/>
-      <c r="V11" s="128"/>
+      <c r="U11" s="131"/>
+      <c r="V11" s="131"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10" t="str">
@@ -15056,11 +15056,11 @@
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
       <c r="E12" s="127"/>
-      <c r="G12" s="135" t="s">
+      <c r="G12" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="129"/>
-      <c r="I12" s="129"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10" t="s">
         <v>71</v>
@@ -15069,17 +15069,17 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="129">
+      <c r="P12" s="128">
         <v>45326</v>
       </c>
-      <c r="Q12" s="129"/>
-      <c r="R12" s="129"/>
+      <c r="Q12" s="128"/>
+      <c r="R12" s="128"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="128">
+      <c r="T12" s="131">
         <v>129</v>
       </c>
-      <c r="U12" s="128"/>
-      <c r="V12" s="128"/>
+      <c r="U12" s="131"/>
+      <c r="V12" s="131"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10" t="str">
@@ -15110,11 +15110,11 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="122"/>
-      <c r="G13" s="135" t="s">
+      <c r="G13" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
         <v>72</v>
@@ -15123,17 +15123,17 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="129">
+      <c r="P13" s="128">
         <v>45325</v>
       </c>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
+      <c r="Q13" s="128"/>
+      <c r="R13" s="128"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="128">
+      <c r="T13" s="131">
         <v>130</v>
       </c>
-      <c r="U13" s="128"/>
-      <c r="V13" s="128"/>
+      <c r="U13" s="131"/>
+      <c r="V13" s="131"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10" t="str">
@@ -15164,11 +15164,11 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="122"/>
-      <c r="G14" s="135" t="s">
+      <c r="G14" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
         <v>73</v>
@@ -15177,17 +15177,17 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="129">
+      <c r="P14" s="128">
         <v>45324</v>
       </c>
-      <c r="Q14" s="129"/>
-      <c r="R14" s="129"/>
+      <c r="Q14" s="128"/>
+      <c r="R14" s="128"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="128">
+      <c r="T14" s="131">
         <v>131</v>
       </c>
-      <c r="U14" s="128"/>
-      <c r="V14" s="128"/>
+      <c r="U14" s="131"/>
+      <c r="V14" s="131"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10" t="str">
@@ -15218,11 +15218,11 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="63"/>
-      <c r="G15" s="135" t="s">
+      <c r="G15" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
         <v>74</v>
@@ -15231,17 +15231,17 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="129">
+      <c r="P15" s="128">
         <v>45323</v>
       </c>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
+      <c r="Q15" s="128"/>
+      <c r="R15" s="128"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="128">
+      <c r="T15" s="131">
         <v>132</v>
       </c>
-      <c r="U15" s="128"/>
-      <c r="V15" s="128"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="131"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10" t="str">
@@ -15272,11 +15272,11 @@
       <c r="C16" s="121"/>
       <c r="D16" s="121"/>
       <c r="E16" s="122"/>
-      <c r="G16" s="135" t="s">
+      <c r="G16" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="129"/>
-      <c r="I16" s="129"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
         <v>75</v>
@@ -15285,17 +15285,17 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="129">
+      <c r="P16" s="128">
         <v>45322</v>
       </c>
-      <c r="Q16" s="129"/>
-      <c r="R16" s="129"/>
+      <c r="Q16" s="128"/>
+      <c r="R16" s="128"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="128">
+      <c r="T16" s="131">
         <v>133</v>
       </c>
-      <c r="U16" s="128"/>
-      <c r="V16" s="128"/>
+      <c r="U16" s="131"/>
+      <c r="V16" s="131"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10" t="str">
@@ -15327,11 +15327,11 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="122"/>
-      <c r="G17" s="135" t="s">
+      <c r="G17" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
         <v>76</v>
@@ -15340,17 +15340,17 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="129">
+      <c r="P17" s="128">
         <v>45321</v>
       </c>
-      <c r="Q17" s="129"/>
-      <c r="R17" s="129"/>
+      <c r="Q17" s="128"/>
+      <c r="R17" s="128"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="128">
+      <c r="T17" s="131">
         <v>134</v>
       </c>
-      <c r="U17" s="128"/>
-      <c r="V17" s="128"/>
+      <c r="U17" s="131"/>
+      <c r="V17" s="131"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10" t="str">
@@ -15381,11 +15381,11 @@
       <c r="C18" s="121"/>
       <c r="D18" s="121"/>
       <c r="E18" s="122"/>
-      <c r="G18" s="135" t="s">
+      <c r="G18" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="129"/>
-      <c r="I18" s="129"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
         <v>77</v>
@@ -15394,17 +15394,17 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="129">
+      <c r="P18" s="128">
         <v>45320</v>
       </c>
-      <c r="Q18" s="129"/>
-      <c r="R18" s="129"/>
+      <c r="Q18" s="128"/>
+      <c r="R18" s="128"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="128">
+      <c r="T18" s="131">
         <v>135</v>
       </c>
-      <c r="U18" s="128"/>
-      <c r="V18" s="128"/>
+      <c r="U18" s="131"/>
+      <c r="V18" s="131"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10" t="str">
@@ -15435,11 +15435,11 @@
       <c r="C19" s="121"/>
       <c r="D19" s="121"/>
       <c r="E19" s="122"/>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="129"/>
-      <c r="I19" s="129"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
         <v>78</v>
@@ -15448,17 +15448,17 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="129">
+      <c r="P19" s="128">
         <v>45319</v>
       </c>
-      <c r="Q19" s="129"/>
-      <c r="R19" s="129"/>
+      <c r="Q19" s="128"/>
+      <c r="R19" s="128"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="128">
+      <c r="T19" s="131">
         <v>136</v>
       </c>
-      <c r="U19" s="128"/>
-      <c r="V19" s="128"/>
+      <c r="U19" s="131"/>
+      <c r="V19" s="131"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10" t="str">
@@ -15489,11 +15489,11 @@
       <c r="C20" s="121"/>
       <c r="D20" s="121"/>
       <c r="E20" s="122"/>
-      <c r="G20" s="135" t="s">
+      <c r="G20" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
         <v>79</v>
@@ -15502,17 +15502,17 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="129">
+      <c r="P20" s="128">
         <v>45318</v>
       </c>
-      <c r="Q20" s="129"/>
-      <c r="R20" s="129"/>
+      <c r="Q20" s="128"/>
+      <c r="R20" s="128"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="128">
+      <c r="T20" s="131">
         <v>137</v>
       </c>
-      <c r="U20" s="128"/>
-      <c r="V20" s="128"/>
+      <c r="U20" s="131"/>
+      <c r="V20" s="131"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10" t="str">
@@ -15543,11 +15543,11 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="122"/>
-      <c r="G21" s="135" t="s">
+      <c r="G21" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="129"/>
-      <c r="I21" s="129"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10" t="s">
         <v>48</v>
@@ -15556,17 +15556,17 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="129">
+      <c r="P21" s="128">
         <v>45317</v>
       </c>
-      <c r="Q21" s="129"/>
-      <c r="R21" s="129"/>
+      <c r="Q21" s="128"/>
+      <c r="R21" s="128"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="128">
+      <c r="T21" s="131">
         <v>138</v>
       </c>
-      <c r="U21" s="128"/>
-      <c r="V21" s="128"/>
+      <c r="U21" s="131"/>
+      <c r="V21" s="131"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10" t="str">
@@ -15597,11 +15597,11 @@
       <c r="C22" s="121"/>
       <c r="D22" s="121"/>
       <c r="E22" s="122"/>
-      <c r="G22" s="135" t="s">
+      <c r="G22" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
         <v>117</v>
@@ -15610,17 +15610,17 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="129">
+      <c r="P22" s="128">
         <v>45316</v>
       </c>
-      <c r="Q22" s="129"/>
-      <c r="R22" s="129"/>
+      <c r="Q22" s="128"/>
+      <c r="R22" s="128"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="128">
+      <c r="T22" s="131">
         <v>139</v>
       </c>
-      <c r="U22" s="128"/>
-      <c r="V22" s="128"/>
+      <c r="U22" s="131"/>
+      <c r="V22" s="131"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10" t="str">
@@ -15651,11 +15651,11 @@
       <c r="C23" s="121"/>
       <c r="D23" s="121"/>
       <c r="E23" s="122"/>
-      <c r="G23" s="135" t="s">
+      <c r="G23" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="129"/>
-      <c r="I23" s="129"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
         <v>12</v>
@@ -15664,17 +15664,17 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="129">
+      <c r="P23" s="128">
         <v>45315</v>
       </c>
-      <c r="Q23" s="129"/>
-      <c r="R23" s="129"/>
+      <c r="Q23" s="128"/>
+      <c r="R23" s="128"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="128">
+      <c r="T23" s="131">
         <v>140</v>
       </c>
-      <c r="U23" s="128"/>
-      <c r="V23" s="128"/>
+      <c r="U23" s="131"/>
+      <c r="V23" s="131"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10" t="str">
@@ -15707,11 +15707,11 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="122"/>
-      <c r="G24" s="135" t="s">
+      <c r="G24" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="129"/>
-      <c r="I24" s="129"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
         <v>84</v>
@@ -15720,17 +15720,17 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="129">
+      <c r="P24" s="128">
         <v>45314</v>
       </c>
-      <c r="Q24" s="129"/>
-      <c r="R24" s="129"/>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="128"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="128">
+      <c r="T24" s="131">
         <v>141</v>
       </c>
-      <c r="U24" s="128"/>
-      <c r="V24" s="128"/>
+      <c r="U24" s="131"/>
+      <c r="V24" s="131"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="str">
@@ -15761,11 +15761,11 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="122"/>
-      <c r="G25" s="135" t="s">
+      <c r="G25" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="129"/>
-      <c r="I25" s="129"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10" t="s">
         <v>69</v>
@@ -15774,17 +15774,17 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="129">
+      <c r="P25" s="128">
         <v>45313</v>
       </c>
-      <c r="Q25" s="129"/>
-      <c r="R25" s="129"/>
+      <c r="Q25" s="128"/>
+      <c r="R25" s="128"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="128">
+      <c r="T25" s="131">
         <v>142</v>
       </c>
-      <c r="U25" s="128"/>
-      <c r="V25" s="128"/>
+      <c r="U25" s="131"/>
+      <c r="V25" s="131"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10" t="str">
@@ -15815,11 +15815,11 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="122"/>
-      <c r="G26" s="135" t="s">
+      <c r="G26" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="129"/>
-      <c r="I26" s="129"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="s">
         <v>70</v>
@@ -15828,17 +15828,17 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="129">
+      <c r="P26" s="128">
         <v>45312</v>
       </c>
-      <c r="Q26" s="129"/>
-      <c r="R26" s="129"/>
+      <c r="Q26" s="128"/>
+      <c r="R26" s="128"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="128">
+      <c r="T26" s="131">
         <v>143</v>
       </c>
-      <c r="U26" s="128"/>
-      <c r="V26" s="128"/>
+      <c r="U26" s="131"/>
+      <c r="V26" s="131"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10" t="str">
@@ -15869,11 +15869,11 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="122"/>
-      <c r="G27" s="135" t="s">
+      <c r="G27" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10" t="s">
         <v>71</v>
@@ -15882,17 +15882,17 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="129">
+      <c r="P27" s="128">
         <v>45311</v>
       </c>
-      <c r="Q27" s="129"/>
-      <c r="R27" s="129"/>
+      <c r="Q27" s="128"/>
+      <c r="R27" s="128"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="128">
+      <c r="T27" s="131">
         <v>144</v>
       </c>
-      <c r="U27" s="128"/>
-      <c r="V27" s="128"/>
+      <c r="U27" s="131"/>
+      <c r="V27" s="131"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10" t="str">
@@ -15923,11 +15923,11 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="122"/>
-      <c r="G28" s="135" t="s">
+      <c r="G28" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="129"/>
-      <c r="I28" s="129"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10" t="s">
         <v>72</v>
@@ -15936,17 +15936,17 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="129">
+      <c r="P28" s="128">
         <v>45310</v>
       </c>
-      <c r="Q28" s="129"/>
-      <c r="R28" s="129"/>
+      <c r="Q28" s="128"/>
+      <c r="R28" s="128"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="128">
+      <c r="T28" s="131">
         <v>145</v>
       </c>
-      <c r="U28" s="128"/>
-      <c r="V28" s="128"/>
+      <c r="U28" s="131"/>
+      <c r="V28" s="131"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10" t="str">
@@ -15977,11 +15977,11 @@
       <c r="C29" s="121"/>
       <c r="D29" s="121"/>
       <c r="E29" s="122"/>
-      <c r="G29" s="135" t="s">
+      <c r="G29" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="129"/>
-      <c r="I29" s="129"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10" t="s">
         <v>73</v>
@@ -15990,17 +15990,17 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="129">
+      <c r="P29" s="128">
         <v>45309</v>
       </c>
-      <c r="Q29" s="129"/>
-      <c r="R29" s="129"/>
+      <c r="Q29" s="128"/>
+      <c r="R29" s="128"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="128">
+      <c r="T29" s="131">
         <v>146</v>
       </c>
-      <c r="U29" s="128"/>
-      <c r="V29" s="128"/>
+      <c r="U29" s="131"/>
+      <c r="V29" s="131"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10" t="str">
@@ -16031,11 +16031,11 @@
       <c r="C30" s="121"/>
       <c r="D30" s="121"/>
       <c r="E30" s="122"/>
-      <c r="G30" s="136" t="s">
+      <c r="G30" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>74</v>
@@ -16044,17 +16044,17 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="131">
+      <c r="P30" s="129">
         <v>45308</v>
       </c>
-      <c r="Q30" s="131"/>
-      <c r="R30" s="131"/>
+      <c r="Q30" s="129"/>
+      <c r="R30" s="129"/>
       <c r="S30" s="2"/>
-      <c r="T30" s="130">
+      <c r="T30" s="132">
         <v>147</v>
       </c>
-      <c r="U30" s="130"/>
-      <c r="V30" s="130"/>
+      <c r="U30" s="132"/>
+      <c r="V30" s="132"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2" t="str">
@@ -16082,43 +16082,48 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="T19:V19"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="T23:V23"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="T25:V25"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="T17:V17"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="T8:V8"/>
     <mergeCell ref="T9:V9"/>
@@ -16135,48 +16140,43 @@
     <mergeCell ref="T30:V30"/>
     <mergeCell ref="P8:R8"/>
     <mergeCell ref="P9:R9"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated mockup for dashboard for transactions, capitalized the labels
</commit_message>
<xml_diff>
--- a/docs/Mockups.xlsx
+++ b/docs/Mockups.xlsx
@@ -1514,14 +1514,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1529,7 +1529,13 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1538,29 +1544,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1569,6 +1566,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1584,18 +1584,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1616,6 +1604,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1624,6 +1621,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1684,14 +1684,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>125027</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>181745</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>167716</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1705,7 +1705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1771650" y="1323975"/>
-          <a:ext cx="8611802" cy="5515745"/>
+          <a:ext cx="7800975" cy="4930216"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3143,12 +3143,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -3503,18 +3503,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="B30:E30"/>
@@ -3531,6 +3519,18 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3628,12 +3628,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -3716,11 +3716,11 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="128">
+      <c r="L8" s="129">
         <v>45336</v>
       </c>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="129"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
         <v>127</v>
@@ -3770,11 +3770,11 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="128">
+      <c r="L9" s="129">
         <v>45324</v>
       </c>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="129"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
         <v>128</v>
@@ -3826,11 +3826,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="128">
+      <c r="L10" s="129">
         <v>45241</v>
       </c>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="129"/>
       <c r="O10" s="10"/>
       <c r="P10" s="9" t="s">
         <v>127</v>
@@ -3880,11 +3880,11 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="128">
+      <c r="L11" s="129">
         <v>45281</v>
       </c>
-      <c r="M11" s="128"/>
-      <c r="N11" s="128"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
         <v>129</v>
@@ -3934,11 +3934,11 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="128">
+      <c r="L12" s="129">
         <v>45220</v>
       </c>
-      <c r="M12" s="128"/>
-      <c r="N12" s="128"/>
+      <c r="M12" s="129"/>
+      <c r="N12" s="129"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
         <v>130</v>
@@ -4737,21 +4737,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -4768,6 +4753,21 @@
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4882,12 +4882,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -5462,17 +5462,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B24:E24"/>
@@ -5489,6 +5478,17 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5586,25 +5586,25 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="N5" s="139" t="s">
+      <c r="N5" s="138" t="s">
         <v>185</v>
       </c>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="141"/>
+      <c r="O5" s="139"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="140"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121" t="s">
@@ -5680,17 +5680,17 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="128">
+      <c r="K8" s="129">
         <v>45353</v>
       </c>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="131">
+      <c r="O8" s="128">
         <v>10</v>
       </c>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="128"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10" t="s">
         <v>127</v>
@@ -5706,9 +5706,9 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
       <c r="AB8" s="10"/>
-      <c r="AC8" s="138"/>
-      <c r="AD8" s="138"/>
-      <c r="AE8" s="138"/>
+      <c r="AC8" s="141"/>
+      <c r="AD8" s="141"/>
+      <c r="AE8" s="141"/>
       <c r="AF8" s="86"/>
       <c r="AG8" s="10" t="s">
         <v>175</v>
@@ -5736,17 +5736,17 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="128">
+      <c r="K9" s="129">
         <v>45353</v>
       </c>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="131">
+      <c r="O9" s="128">
         <v>10</v>
       </c>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="128"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10" t="s">
         <v>127</v>
@@ -5762,9 +5762,9 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
-      <c r="AC9" s="138"/>
-      <c r="AD9" s="138"/>
-      <c r="AE9" s="138"/>
+      <c r="AC9" s="141"/>
+      <c r="AD9" s="141"/>
+      <c r="AE9" s="141"/>
       <c r="AF9" s="86"/>
       <c r="AG9" s="10" t="s">
         <v>175</v>
@@ -5788,13 +5788,13 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="128"/>
+      <c r="Q10" s="128"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5806,9 +5806,9 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
-      <c r="AC10" s="138"/>
-      <c r="AD10" s="138"/>
-      <c r="AE10" s="138"/>
+      <c r="AC10" s="141"/>
+      <c r="AD10" s="141"/>
+      <c r="AE10" s="141"/>
       <c r="AF10" s="86"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="86"/>
@@ -5834,17 +5834,17 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="128">
+      <c r="K11" s="129">
         <v>45354</v>
       </c>
-      <c r="L11" s="128"/>
-      <c r="M11" s="128"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="131">
+      <c r="O11" s="128">
         <v>5</v>
       </c>
-      <c r="P11" s="131"/>
-      <c r="Q11" s="131"/>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="128"/>
       <c r="R11" s="10"/>
       <c r="S11" s="9" t="s">
         <v>130</v>
@@ -5860,9 +5860,9 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
-      <c r="AC11" s="138"/>
-      <c r="AD11" s="138"/>
-      <c r="AE11" s="138"/>
+      <c r="AC11" s="141"/>
+      <c r="AD11" s="141"/>
+      <c r="AE11" s="141"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="9" t="s">
         <v>176</v>
@@ -5888,17 +5888,17 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="128">
+      <c r="K12" s="129">
         <v>45355</v>
       </c>
-      <c r="L12" s="128"/>
-      <c r="M12" s="128"/>
+      <c r="L12" s="129"/>
+      <c r="M12" s="129"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="131">
+      <c r="O12" s="128">
         <v>10</v>
       </c>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="131"/>
+      <c r="P12" s="128"/>
+      <c r="Q12" s="128"/>
       <c r="R12" s="10"/>
       <c r="S12" s="9" t="s">
         <v>128</v>
@@ -5944,17 +5944,17 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="128">
+      <c r="K13" s="129">
         <v>45356</v>
       </c>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="131">
+      <c r="O13" s="128">
         <v>20</v>
       </c>
-      <c r="P13" s="131"/>
-      <c r="Q13" s="131"/>
+      <c r="P13" s="128"/>
+      <c r="Q13" s="128"/>
       <c r="R13" s="10"/>
       <c r="S13" s="9" t="s">
         <v>129</v>
@@ -6187,26 +6187,26 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="131">
+      <c r="M21" s="128">
         <v>30</v>
       </c>
-      <c r="N21" s="131"/>
-      <c r="O21" s="131"/>
+      <c r="N21" s="128"/>
+      <c r="O21" s="128"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="131">
+      <c r="Q21" s="128">
         <v>35</v>
       </c>
-      <c r="R21" s="131"/>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
+      <c r="R21" s="128"/>
+      <c r="S21" s="128"/>
+      <c r="T21" s="128"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="131">
+      <c r="V21" s="128">
         <f>M21-Q21</f>
         <v>-5</v>
       </c>
-      <c r="W21" s="131"/>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="131"/>
+      <c r="W21" s="128"/>
+      <c r="X21" s="128"/>
+      <c r="Y21" s="128"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="44"/>
     </row>
@@ -6223,26 +6223,26 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="131">
+      <c r="M22" s="128">
         <v>20</v>
       </c>
-      <c r="N22" s="131"/>
-      <c r="O22" s="131"/>
+      <c r="N22" s="128"/>
+      <c r="O22" s="128"/>
       <c r="P22" s="10"/>
-      <c r="Q22" s="131">
+      <c r="Q22" s="128">
         <v>10</v>
       </c>
-      <c r="R22" s="131"/>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
+      <c r="R22" s="128"/>
+      <c r="S22" s="128"/>
+      <c r="T22" s="128"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="131">
+      <c r="V22" s="128">
         <f>M22-Q22</f>
         <v>10</v>
       </c>
-      <c r="W22" s="131"/>
-      <c r="X22" s="131"/>
-      <c r="Y22" s="131"/>
+      <c r="W22" s="128"/>
+      <c r="X22" s="128"/>
+      <c r="Y22" s="128"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="44"/>
     </row>
@@ -6259,26 +6259,26 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="131">
+      <c r="M23" s="128">
         <v>5</v>
       </c>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
+      <c r="N23" s="128"/>
+      <c r="O23" s="128"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="131">
+      <c r="Q23" s="128">
         <v>10</v>
       </c>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
+      <c r="R23" s="128"/>
+      <c r="S23" s="128"/>
+      <c r="T23" s="128"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="131">
+      <c r="V23" s="128">
         <f>M23-Q23</f>
         <v>-5</v>
       </c>
-      <c r="W23" s="131"/>
-      <c r="X23" s="131"/>
-      <c r="Y23" s="131"/>
+      <c r="W23" s="128"/>
+      <c r="X23" s="128"/>
+      <c r="Y23" s="128"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="44"/>
     </row>
@@ -6295,26 +6295,26 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="131">
+      <c r="M24" s="128">
         <v>10</v>
       </c>
-      <c r="N24" s="131"/>
-      <c r="O24" s="131"/>
+      <c r="N24" s="128"/>
+      <c r="O24" s="128"/>
       <c r="P24" s="10"/>
-      <c r="Q24" s="131">
+      <c r="Q24" s="128">
         <v>10</v>
       </c>
-      <c r="R24" s="131"/>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
+      <c r="R24" s="128"/>
+      <c r="S24" s="128"/>
+      <c r="T24" s="128"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="131">
+      <c r="V24" s="128">
         <f>M24-Q24</f>
         <v>0</v>
       </c>
-      <c r="W24" s="131"/>
-      <c r="X24" s="131"/>
-      <c r="Y24" s="131"/>
+      <c r="W24" s="128"/>
+      <c r="X24" s="128"/>
+      <c r="Y24" s="128"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="44"/>
     </row>
@@ -6380,15 +6380,36 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="Q21:T21"/>
-    <mergeCell ref="Q22:T22"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="AC11:AE11"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="AC10:AE10"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="M21:O21"/>
@@ -6405,36 +6426,15 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="AC11:AE11"/>
-    <mergeCell ref="AC9:AE9"/>
-    <mergeCell ref="AC10:AE10"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V23:Y23"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="Q22:T22"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q24:T24"/>
   </mergeCells>
   <conditionalFormatting sqref="V21:Y24">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -6559,12 +6559,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -7083,20 +7083,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="H8:R8"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -7113,6 +7099,20 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7517,10 +7517,10 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="44"/>
-      <c r="J46" s="139" t="s">
+      <c r="J46" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="K46" s="141"/>
+      <c r="K46" s="140"/>
       <c r="M46" s="144"/>
       <c r="N46" s="144"/>
       <c r="O46" s="144"/>
@@ -7939,46 +7939,46 @@
       <c r="C5" s="121"/>
       <c r="D5" s="121"/>
       <c r="E5" s="146"/>
-      <c r="G5" s="147" t="s">
+      <c r="G5" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="147"/>
-      <c r="AI5" s="147"/>
-      <c r="AJ5" s="147"/>
-      <c r="AK5" s="147"/>
-      <c r="AL5" s="147"/>
-      <c r="AM5" s="147"/>
-      <c r="AN5" s="147"/>
-      <c r="AO5" s="147"/>
-      <c r="AP5" s="147"/>
-      <c r="AQ5" s="147"/>
-      <c r="AR5" s="147"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="159"/>
+      <c r="AK5" s="159"/>
+      <c r="AL5" s="159"/>
+      <c r="AM5" s="159"/>
+      <c r="AN5" s="159"/>
+      <c r="AO5" s="159"/>
+      <c r="AP5" s="159"/>
+      <c r="AQ5" s="159"/>
+      <c r="AR5" s="159"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -8095,13 +8095,13 @@
       <c r="C8" s="121"/>
       <c r="D8" s="121"/>
       <c r="E8" s="146"/>
-      <c r="G8" s="157" t="s">
+      <c r="G8" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="158"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="159"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="157"/>
+      <c r="K8" s="158"/>
       <c r="L8" s="25" t="s">
         <v>25</v>
       </c>
@@ -8210,13 +8210,13 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="146"/>
-      <c r="G9" s="148" t="s">
+      <c r="G9" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="149"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="149"/>
-      <c r="K9" s="150"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="155"/>
       <c r="L9" s="24">
         <f t="shared" ref="L9:M12" si="0">SUM(M9:AQ9)</f>
         <v>610</v>
@@ -8324,13 +8324,13 @@
       <c r="C10" s="121"/>
       <c r="D10" s="121"/>
       <c r="E10" s="146"/>
-      <c r="G10" s="148" t="s">
+      <c r="G10" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="149"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="150"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="155"/>
       <c r="L10" s="24">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -8380,13 +8380,13 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="146"/>
-      <c r="G11" s="148" t="s">
+      <c r="G11" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="149"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="149"/>
-      <c r="K11" s="150"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="155"/>
       <c r="L11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8432,13 +8432,13 @@
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
       <c r="E12" s="146"/>
-      <c r="G12" s="148" t="s">
+      <c r="G12" s="153" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="150"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="155"/>
       <c r="L12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8484,13 +8484,13 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="146"/>
-      <c r="G13" s="148" t="s">
+      <c r="G13" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="149"/>
-      <c r="K13" s="150"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
+      <c r="K13" s="155"/>
       <c r="L13" s="24">
         <v>500</v>
       </c>
@@ -8541,13 +8541,13 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="146"/>
-      <c r="G14" s="148" t="s">
+      <c r="G14" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="149"/>
-      <c r="I14" s="149"/>
-      <c r="J14" s="149"/>
-      <c r="K14" s="150"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="155"/>
       <c r="L14" s="24">
         <f>SUM(M14:AQ14)</f>
         <v>246</v>
@@ -8595,13 +8595,13 @@
       <c r="C15" s="121"/>
       <c r="D15" s="121"/>
       <c r="E15" s="146"/>
-      <c r="G15" s="148" t="s">
+      <c r="G15" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="149"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="149"/>
-      <c r="K15" s="150"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="155"/>
       <c r="L15" s="24">
         <f>SUM(M15:AQ15)</f>
         <v>220</v>
@@ -8649,13 +8649,13 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="G16" s="151" t="s">
+      <c r="G16" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="152"/>
-      <c r="I16" s="152"/>
-      <c r="J16" s="152"/>
-      <c r="K16" s="153"/>
+      <c r="H16" s="148"/>
+      <c r="I16" s="148"/>
+      <c r="J16" s="148"/>
+      <c r="K16" s="149"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="11"/>
@@ -8695,13 +8695,13 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="146"/>
-      <c r="G17" s="154" t="s">
+      <c r="G17" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="155"/>
-      <c r="I17" s="155"/>
-      <c r="J17" s="155"/>
-      <c r="K17" s="156"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="26">
         <f>SUM(L9:L16)</f>
         <v>1976</v>
@@ -8863,46 +8863,46 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="146"/>
-      <c r="G21" s="147" t="s">
+      <c r="G21" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="147"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="147"/>
-      <c r="K21" s="147"/>
-      <c r="L21" s="147"/>
-      <c r="M21" s="147"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="147"/>
-      <c r="P21" s="147"/>
-      <c r="Q21" s="147"/>
-      <c r="R21" s="147"/>
-      <c r="S21" s="147"/>
-      <c r="T21" s="147"/>
-      <c r="U21" s="147"/>
-      <c r="V21" s="147"/>
-      <c r="W21" s="147"/>
-      <c r="X21" s="147"/>
-      <c r="Y21" s="147"/>
-      <c r="Z21" s="147"/>
-      <c r="AA21" s="147"/>
-      <c r="AB21" s="147"/>
-      <c r="AC21" s="147"/>
-      <c r="AD21" s="147"/>
-      <c r="AE21" s="147"/>
-      <c r="AF21" s="147"/>
-      <c r="AG21" s="147"/>
-      <c r="AH21" s="147"/>
-      <c r="AI21" s="147"/>
-      <c r="AJ21" s="147"/>
-      <c r="AK21" s="147"/>
-      <c r="AL21" s="147"/>
-      <c r="AM21" s="147"/>
-      <c r="AN21" s="147"/>
-      <c r="AO21" s="147"/>
-      <c r="AP21" s="147"/>
-      <c r="AQ21" s="147"/>
-      <c r="AR21" s="147"/>
+      <c r="H21" s="159"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="159"/>
+      <c r="K21" s="159"/>
+      <c r="L21" s="159"/>
+      <c r="M21" s="159"/>
+      <c r="N21" s="159"/>
+      <c r="O21" s="159"/>
+      <c r="P21" s="159"/>
+      <c r="Q21" s="159"/>
+      <c r="R21" s="159"/>
+      <c r="S21" s="159"/>
+      <c r="T21" s="159"/>
+      <c r="U21" s="159"/>
+      <c r="V21" s="159"/>
+      <c r="W21" s="159"/>
+      <c r="X21" s="159"/>
+      <c r="Y21" s="159"/>
+      <c r="Z21" s="159"/>
+      <c r="AA21" s="159"/>
+      <c r="AB21" s="159"/>
+      <c r="AC21" s="159"/>
+      <c r="AD21" s="159"/>
+      <c r="AE21" s="159"/>
+      <c r="AF21" s="159"/>
+      <c r="AG21" s="159"/>
+      <c r="AH21" s="159"/>
+      <c r="AI21" s="159"/>
+      <c r="AJ21" s="159"/>
+      <c r="AK21" s="159"/>
+      <c r="AL21" s="159"/>
+      <c r="AM21" s="159"/>
+      <c r="AN21" s="159"/>
+      <c r="AO21" s="159"/>
+      <c r="AP21" s="159"/>
+      <c r="AQ21" s="159"/>
+      <c r="AR21" s="159"/>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B22" s="121"/>
@@ -9015,13 +9015,13 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="146"/>
-      <c r="G24" s="157" t="s">
+      <c r="G24" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="158"/>
-      <c r="K24" s="159"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="158"/>
       <c r="L24" s="25" t="s">
         <v>25</v>
       </c>
@@ -9127,13 +9127,13 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="146"/>
-      <c r="G25" s="148" t="s">
+      <c r="G25" s="153" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="149"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="150"/>
+      <c r="H25" s="154"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="154"/>
+      <c r="K25" s="155"/>
       <c r="L25" s="24">
         <f>SUM(M25:AQ25)</f>
         <v>610</v>
@@ -9241,13 +9241,13 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="146"/>
-      <c r="G26" s="148" t="s">
+      <c r="G26" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="150"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="154"/>
+      <c r="K26" s="155"/>
       <c r="L26" s="24">
         <f>SUM(M26:AQ26)</f>
         <v>400</v>
@@ -9297,13 +9297,13 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="146"/>
-      <c r="G27" s="151" t="s">
+      <c r="G27" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="152"/>
-      <c r="K27" s="153"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
+      <c r="K27" s="149"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="11"/>
@@ -9343,13 +9343,13 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="146"/>
-      <c r="G28" s="154" t="s">
+      <c r="G28" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="155"/>
-      <c r="I28" s="155"/>
-      <c r="J28" s="155"/>
-      <c r="K28" s="156"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="151"/>
+      <c r="K28" s="152"/>
       <c r="L28" s="26">
         <f>SUM(L25:L27)</f>
         <v>1010</v>
@@ -9507,24 +9507,15 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G21:AR21"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="G5:AR5"/>
     <mergeCell ref="G9:K9"/>
@@ -9541,15 +9532,24 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G21:AR21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:L16">
     <cfRule type="dataBar" priority="2">
@@ -9708,43 +9708,43 @@
       <c r="G5" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="147"/>
-      <c r="AI5" s="147"/>
-      <c r="AJ5" s="147"/>
-      <c r="AK5" s="147"/>
-      <c r="AL5" s="147"/>
-      <c r="AM5" s="147"/>
-      <c r="AN5" s="147"/>
-      <c r="AO5" s="147"/>
-      <c r="AP5" s="147"/>
-      <c r="AQ5" s="147"/>
-      <c r="AR5" s="147"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="159"/>
+      <c r="AK5" s="159"/>
+      <c r="AL5" s="159"/>
+      <c r="AM5" s="159"/>
+      <c r="AN5" s="159"/>
+      <c r="AO5" s="159"/>
+      <c r="AP5" s="159"/>
+      <c r="AQ5" s="159"/>
+      <c r="AR5" s="159"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -9753,11 +9753,11 @@
       <c r="E6" s="146"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="161"/>
       <c r="G7" s="40" t="s">
         <v>28</v>
@@ -10216,23 +10216,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:AR5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:AR5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11217,7 +11217,7 @@
   <dimension ref="B2:AS33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BB27" sqref="BB27"/>
+      <selection activeCell="AV29" sqref="AV29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11306,24 +11306,24 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="G5" s="120" t="s">
         <v>168</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="123" t="s">
+      <c r="K5" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
@@ -11500,20 +11500,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B31:E31"/>
@@ -11530,6 +11516,20 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:N5">
@@ -11643,12 +11643,12 @@
       <c r="E5" s="122"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -11798,12 +11798,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -11816,14 +11818,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11922,12 +11922,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -12846,12 +12846,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -12864,14 +12866,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12983,12 +12983,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -13229,12 +13229,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -13247,14 +13249,12 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13352,12 +13352,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -13387,11 +13387,11 @@
       <c r="K7" s="68"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="130" t="s">
+      <c r="N7" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
       <c r="Q7" s="68"/>
       <c r="R7" s="68" t="s">
         <v>25</v>
@@ -13428,17 +13428,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="128">
+      <c r="N8" s="129">
         <v>45334</v>
       </c>
-      <c r="O8" s="128"/>
-      <c r="P8" s="128"/>
+      <c r="O8" s="129"/>
+      <c r="P8" s="129"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="131">
+      <c r="R8" s="128">
         <v>500</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
+      <c r="S8" s="128"/>
+      <c r="T8" s="128"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -13460,17 +13460,17 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="128">
+      <c r="N9" s="129">
         <v>45334</v>
       </c>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
+      <c r="O9" s="129"/>
+      <c r="P9" s="129"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="131">
+      <c r="R9" s="128">
         <v>501</v>
       </c>
-      <c r="S9" s="131"/>
-      <c r="T9" s="131"/>
+      <c r="S9" s="128"/>
+      <c r="T9" s="128"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -13492,17 +13492,17 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="128">
+      <c r="N10" s="129">
         <v>45334</v>
       </c>
-      <c r="O10" s="128"/>
-      <c r="P10" s="128"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="129"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="131">
+      <c r="R10" s="128">
         <v>502</v>
       </c>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
+      <c r="S10" s="128"/>
+      <c r="T10" s="128"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -13524,17 +13524,17 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="128">
+      <c r="N11" s="129">
         <v>45334</v>
       </c>
-      <c r="O11" s="128"/>
-      <c r="P11" s="128"/>
+      <c r="O11" s="129"/>
+      <c r="P11" s="129"/>
       <c r="Q11" s="10"/>
-      <c r="R11" s="131">
+      <c r="R11" s="128">
         <v>503</v>
       </c>
-      <c r="S11" s="131"/>
-      <c r="T11" s="131"/>
+      <c r="S11" s="128"/>
+      <c r="T11" s="128"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -13556,17 +13556,17 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="128">
+      <c r="N12" s="129">
         <v>45334</v>
       </c>
-      <c r="O12" s="128"/>
-      <c r="P12" s="128"/>
+      <c r="O12" s="129"/>
+      <c r="P12" s="129"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="131">
+      <c r="R12" s="128">
         <v>504</v>
       </c>
-      <c r="S12" s="131"/>
-      <c r="T12" s="131"/>
+      <c r="S12" s="128"/>
+      <c r="T12" s="128"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -13588,17 +13588,17 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="128">
+      <c r="N13" s="129">
         <v>45334</v>
       </c>
-      <c r="O13" s="128"/>
-      <c r="P13" s="128"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
       <c r="Q13" s="10"/>
-      <c r="R13" s="131">
+      <c r="R13" s="128">
         <v>505</v>
       </c>
-      <c r="S13" s="131"/>
-      <c r="T13" s="131"/>
+      <c r="S13" s="128"/>
+      <c r="T13" s="128"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -13620,17 +13620,17 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="128">
+      <c r="N14" s="129">
         <v>45334</v>
       </c>
-      <c r="O14" s="128"/>
-      <c r="P14" s="128"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="129"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="131">
+      <c r="R14" s="128">
         <v>506</v>
       </c>
-      <c r="S14" s="131"/>
-      <c r="T14" s="131"/>
+      <c r="S14" s="128"/>
+      <c r="T14" s="128"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -13652,17 +13652,17 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="128">
+      <c r="N15" s="129">
         <v>45334</v>
       </c>
-      <c r="O15" s="128"/>
-      <c r="P15" s="128"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="129"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="131">
+      <c r="R15" s="128">
         <v>507</v>
       </c>
-      <c r="S15" s="131"/>
-      <c r="T15" s="131"/>
+      <c r="S15" s="128"/>
+      <c r="T15" s="128"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
@@ -13684,17 +13684,17 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="128">
+      <c r="N16" s="129">
         <v>45334</v>
       </c>
-      <c r="O16" s="128"/>
-      <c r="P16" s="128"/>
+      <c r="O16" s="129"/>
+      <c r="P16" s="129"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="131">
+      <c r="R16" s="128">
         <v>508</v>
       </c>
-      <c r="S16" s="131"/>
-      <c r="T16" s="131"/>
+      <c r="S16" s="128"/>
+      <c r="T16" s="128"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -13717,17 +13717,17 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="128">
+      <c r="N17" s="129">
         <v>45334</v>
       </c>
-      <c r="O17" s="128"/>
-      <c r="P17" s="128"/>
+      <c r="O17" s="129"/>
+      <c r="P17" s="129"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="131">
+      <c r="R17" s="128">
         <v>509</v>
       </c>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
+      <c r="S17" s="128"/>
+      <c r="T17" s="128"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -13749,17 +13749,17 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="128">
+      <c r="N18" s="129">
         <v>45334</v>
       </c>
-      <c r="O18" s="128"/>
-      <c r="P18" s="128"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="129"/>
       <c r="Q18" s="10"/>
-      <c r="R18" s="131">
+      <c r="R18" s="128">
         <v>510</v>
       </c>
-      <c r="S18" s="131"/>
-      <c r="T18" s="131"/>
+      <c r="S18" s="128"/>
+      <c r="T18" s="128"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
@@ -13781,17 +13781,17 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="128">
+      <c r="N19" s="129">
         <v>45334</v>
       </c>
-      <c r="O19" s="128"/>
-      <c r="P19" s="128"/>
+      <c r="O19" s="129"/>
+      <c r="P19" s="129"/>
       <c r="Q19" s="10"/>
-      <c r="R19" s="131">
+      <c r="R19" s="128">
         <v>511</v>
       </c>
-      <c r="S19" s="131"/>
-      <c r="T19" s="131"/>
+      <c r="S19" s="128"/>
+      <c r="T19" s="128"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -13813,17 +13813,17 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="128">
+      <c r="N20" s="129">
         <v>45334</v>
       </c>
-      <c r="O20" s="128"/>
-      <c r="P20" s="128"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="129"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="131">
+      <c r="R20" s="128">
         <v>512</v>
       </c>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
+      <c r="S20" s="128"/>
+      <c r="T20" s="128"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
@@ -13845,17 +13845,17 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="128">
+      <c r="N21" s="129">
         <v>45292</v>
       </c>
-      <c r="O21" s="128"/>
-      <c r="P21" s="128"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="129"/>
       <c r="Q21" s="10"/>
-      <c r="R21" s="131">
+      <c r="R21" s="128">
         <v>513</v>
       </c>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
+      <c r="S21" s="128"/>
+      <c r="T21" s="128"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -13877,17 +13877,17 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="128">
+      <c r="N22" s="129">
         <v>45292</v>
       </c>
-      <c r="O22" s="128"/>
-      <c r="P22" s="128"/>
+      <c r="O22" s="129"/>
+      <c r="P22" s="129"/>
       <c r="Q22" s="10"/>
-      <c r="R22" s="131">
+      <c r="R22" s="128">
         <v>514</v>
       </c>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
+      <c r="S22" s="128"/>
+      <c r="T22" s="128"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
@@ -13909,17 +13909,17 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="128">
+      <c r="N23" s="129">
         <v>45292</v>
       </c>
-      <c r="O23" s="128"/>
-      <c r="P23" s="128"/>
+      <c r="O23" s="129"/>
+      <c r="P23" s="129"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="131">
+      <c r="R23" s="128">
         <v>515</v>
       </c>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
+      <c r="S23" s="128"/>
+      <c r="T23" s="128"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -13941,17 +13941,17 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="128">
+      <c r="N24" s="129">
         <v>45292</v>
       </c>
-      <c r="O24" s="128"/>
-      <c r="P24" s="128"/>
+      <c r="O24" s="129"/>
+      <c r="P24" s="129"/>
       <c r="Q24" s="10"/>
-      <c r="R24" s="131">
+      <c r="R24" s="128">
         <v>516</v>
       </c>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
+      <c r="S24" s="128"/>
+      <c r="T24" s="128"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -13973,17 +13973,17 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="128">
+      <c r="N25" s="129">
         <v>45292</v>
       </c>
-      <c r="O25" s="128"/>
-      <c r="P25" s="128"/>
+      <c r="O25" s="129"/>
+      <c r="P25" s="129"/>
       <c r="Q25" s="10"/>
-      <c r="R25" s="131">
+      <c r="R25" s="128">
         <v>517</v>
       </c>
-      <c r="S25" s="131"/>
-      <c r="T25" s="131"/>
+      <c r="S25" s="128"/>
+      <c r="T25" s="128"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -14005,17 +14005,17 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="128">
+      <c r="N26" s="129">
         <v>45292</v>
       </c>
-      <c r="O26" s="128"/>
-      <c r="P26" s="128"/>
+      <c r="O26" s="129"/>
+      <c r="P26" s="129"/>
       <c r="Q26" s="10"/>
-      <c r="R26" s="131">
+      <c r="R26" s="128">
         <v>518</v>
       </c>
-      <c r="S26" s="131"/>
-      <c r="T26" s="131"/>
+      <c r="S26" s="128"/>
+      <c r="T26" s="128"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -14037,17 +14037,17 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="128">
+      <c r="N27" s="129">
         <v>45292</v>
       </c>
-      <c r="O27" s="128"/>
-      <c r="P27" s="128"/>
+      <c r="O27" s="129"/>
+      <c r="P27" s="129"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="131">
+      <c r="R27" s="128">
         <v>519</v>
       </c>
-      <c r="S27" s="131"/>
-      <c r="T27" s="131"/>
+      <c r="S27" s="128"/>
+      <c r="T27" s="128"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
@@ -14069,17 +14069,17 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="128">
+      <c r="N28" s="129">
         <v>45292</v>
       </c>
-      <c r="O28" s="128"/>
-      <c r="P28" s="128"/>
+      <c r="O28" s="129"/>
+      <c r="P28" s="129"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="131">
+      <c r="R28" s="128">
         <v>520</v>
       </c>
-      <c r="S28" s="131"/>
-      <c r="T28" s="131"/>
+      <c r="S28" s="128"/>
+      <c r="T28" s="128"/>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
@@ -14101,17 +14101,17 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="128">
+      <c r="N29" s="129">
         <v>45292</v>
       </c>
-      <c r="O29" s="128"/>
-      <c r="P29" s="128"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="131">
+      <c r="R29" s="128">
         <v>521</v>
       </c>
-      <c r="S29" s="131"/>
-      <c r="T29" s="131"/>
+      <c r="S29" s="128"/>
+      <c r="T29" s="128"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
@@ -14133,17 +14133,17 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="129">
+      <c r="N30" s="131">
         <v>45292</v>
       </c>
-      <c r="O30" s="129"/>
-      <c r="P30" s="129"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="132">
+      <c r="R30" s="130">
         <v>522</v>
       </c>
-      <c r="S30" s="132"/>
-      <c r="T30" s="132"/>
+      <c r="S30" s="130"/>
+      <c r="T30" s="130"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -14153,24 +14153,45 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R21:T21"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="R8:T8"/>
@@ -14187,45 +14208,24 @@
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14337,12 +14337,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -14631,18 +14631,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H12:J12"/>
@@ -14659,6 +14647,18 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14758,12 +14758,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -14838,11 +14838,11 @@
       <c r="C8" s="126"/>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
-      <c r="G8" s="136" t="s">
+      <c r="G8" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="128"/>
-      <c r="I8" s="128"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10" t="s">
         <v>12</v>
@@ -14851,17 +14851,17 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="128">
+      <c r="P8" s="129">
         <v>45330</v>
       </c>
-      <c r="Q8" s="128"/>
-      <c r="R8" s="128"/>
+      <c r="Q8" s="129"/>
+      <c r="R8" s="129"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="131">
+      <c r="T8" s="128">
         <v>125</v>
       </c>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10" t="str">
@@ -14892,11 +14892,11 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="122"/>
-      <c r="G9" s="136" t="s">
+      <c r="G9" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="128"/>
-      <c r="I9" s="128"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>84</v>
@@ -14905,17 +14905,17 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="128">
+      <c r="P9" s="129">
         <v>45329</v>
       </c>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="128"/>
+      <c r="Q9" s="129"/>
+      <c r="R9" s="129"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="131">
+      <c r="T9" s="128">
         <v>120</v>
       </c>
-      <c r="U9" s="131"/>
-      <c r="V9" s="131"/>
+      <c r="U9" s="128"/>
+      <c r="V9" s="128"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10" t="str">
@@ -14948,11 +14948,11 @@
       <c r="C10" s="126"/>
       <c r="D10" s="126"/>
       <c r="E10" s="127"/>
-      <c r="G10" s="136" t="s">
+      <c r="G10" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
         <v>69</v>
@@ -14961,17 +14961,17 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="128">
+      <c r="P10" s="129">
         <v>45328</v>
       </c>
-      <c r="Q10" s="128"/>
-      <c r="R10" s="128"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="129"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="131">
+      <c r="T10" s="128">
         <v>127</v>
       </c>
-      <c r="U10" s="131"/>
-      <c r="V10" s="131"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10" t="str">
@@ -15002,11 +15002,11 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="122"/>
-      <c r="G11" s="136" t="s">
+      <c r="G11" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
         <v>70</v>
@@ -15015,17 +15015,17 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="128">
+      <c r="P11" s="129">
         <v>45327</v>
       </c>
-      <c r="Q11" s="128"/>
-      <c r="R11" s="128"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="131">
+      <c r="T11" s="128">
         <v>128</v>
       </c>
-      <c r="U11" s="131"/>
-      <c r="V11" s="131"/>
+      <c r="U11" s="128"/>
+      <c r="V11" s="128"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10" t="str">
@@ -15056,11 +15056,11 @@
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
       <c r="E12" s="127"/>
-      <c r="G12" s="136" t="s">
+      <c r="G12" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10" t="s">
         <v>71</v>
@@ -15069,17 +15069,17 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="128">
+      <c r="P12" s="129">
         <v>45326</v>
       </c>
-      <c r="Q12" s="128"/>
-      <c r="R12" s="128"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="129"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="131">
+      <c r="T12" s="128">
         <v>129</v>
       </c>
-      <c r="U12" s="131"/>
-      <c r="V12" s="131"/>
+      <c r="U12" s="128"/>
+      <c r="V12" s="128"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10" t="str">
@@ -15110,11 +15110,11 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="122"/>
-      <c r="G13" s="136" t="s">
+      <c r="G13" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
         <v>72</v>
@@ -15123,17 +15123,17 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="128">
+      <c r="P13" s="129">
         <v>45325</v>
       </c>
-      <c r="Q13" s="128"/>
-      <c r="R13" s="128"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="129"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="131">
+      <c r="T13" s="128">
         <v>130</v>
       </c>
-      <c r="U13" s="131"/>
-      <c r="V13" s="131"/>
+      <c r="U13" s="128"/>
+      <c r="V13" s="128"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10" t="str">
@@ -15164,11 +15164,11 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="122"/>
-      <c r="G14" s="136" t="s">
+      <c r="G14" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
         <v>73</v>
@@ -15177,17 +15177,17 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="128">
+      <c r="P14" s="129">
         <v>45324</v>
       </c>
-      <c r="Q14" s="128"/>
-      <c r="R14" s="128"/>
+      <c r="Q14" s="129"/>
+      <c r="R14" s="129"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="131">
+      <c r="T14" s="128">
         <v>131</v>
       </c>
-      <c r="U14" s="131"/>
-      <c r="V14" s="131"/>
+      <c r="U14" s="128"/>
+      <c r="V14" s="128"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10" t="str">
@@ -15218,11 +15218,11 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="63"/>
-      <c r="G15" s="136" t="s">
+      <c r="G15" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
         <v>74</v>
@@ -15231,17 +15231,17 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="128">
+      <c r="P15" s="129">
         <v>45323</v>
       </c>
-      <c r="Q15" s="128"/>
-      <c r="R15" s="128"/>
+      <c r="Q15" s="129"/>
+      <c r="R15" s="129"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="131">
+      <c r="T15" s="128">
         <v>132</v>
       </c>
-      <c r="U15" s="131"/>
-      <c r="V15" s="131"/>
+      <c r="U15" s="128"/>
+      <c r="V15" s="128"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10" t="str">
@@ -15272,11 +15272,11 @@
       <c r="C16" s="121"/>
       <c r="D16" s="121"/>
       <c r="E16" s="122"/>
-      <c r="G16" s="136" t="s">
+      <c r="G16" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="128"/>
-      <c r="I16" s="128"/>
+      <c r="H16" s="129"/>
+      <c r="I16" s="129"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
         <v>75</v>
@@ -15285,17 +15285,17 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="128">
+      <c r="P16" s="129">
         <v>45322</v>
       </c>
-      <c r="Q16" s="128"/>
-      <c r="R16" s="128"/>
+      <c r="Q16" s="129"/>
+      <c r="R16" s="129"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="131">
+      <c r="T16" s="128">
         <v>133</v>
       </c>
-      <c r="U16" s="131"/>
-      <c r="V16" s="131"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10" t="str">
@@ -15327,11 +15327,11 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="122"/>
-      <c r="G17" s="136" t="s">
+      <c r="G17" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
         <v>76</v>
@@ -15340,17 +15340,17 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="128">
+      <c r="P17" s="129">
         <v>45321</v>
       </c>
-      <c r="Q17" s="128"/>
-      <c r="R17" s="128"/>
+      <c r="Q17" s="129"/>
+      <c r="R17" s="129"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="131">
+      <c r="T17" s="128">
         <v>134</v>
       </c>
-      <c r="U17" s="131"/>
-      <c r="V17" s="131"/>
+      <c r="U17" s="128"/>
+      <c r="V17" s="128"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10" t="str">
@@ -15381,11 +15381,11 @@
       <c r="C18" s="121"/>
       <c r="D18" s="121"/>
       <c r="E18" s="122"/>
-      <c r="G18" s="136" t="s">
+      <c r="G18" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="128"/>
-      <c r="I18" s="128"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="129"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
         <v>77</v>
@@ -15394,17 +15394,17 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="128">
+      <c r="P18" s="129">
         <v>45320</v>
       </c>
-      <c r="Q18" s="128"/>
-      <c r="R18" s="128"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="129"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="131">
+      <c r="T18" s="128">
         <v>135</v>
       </c>
-      <c r="U18" s="131"/>
-      <c r="V18" s="131"/>
+      <c r="U18" s="128"/>
+      <c r="V18" s="128"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10" t="str">
@@ -15435,11 +15435,11 @@
       <c r="C19" s="121"/>
       <c r="D19" s="121"/>
       <c r="E19" s="122"/>
-      <c r="G19" s="136" t="s">
+      <c r="G19" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
         <v>78</v>
@@ -15448,17 +15448,17 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="128">
+      <c r="P19" s="129">
         <v>45319</v>
       </c>
-      <c r="Q19" s="128"/>
-      <c r="R19" s="128"/>
+      <c r="Q19" s="129"/>
+      <c r="R19" s="129"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="131">
+      <c r="T19" s="128">
         <v>136</v>
       </c>
-      <c r="U19" s="131"/>
-      <c r="V19" s="131"/>
+      <c r="U19" s="128"/>
+      <c r="V19" s="128"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10" t="str">
@@ -15489,11 +15489,11 @@
       <c r="C20" s="121"/>
       <c r="D20" s="121"/>
       <c r="E20" s="122"/>
-      <c r="G20" s="136" t="s">
+      <c r="G20" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="128"/>
-      <c r="I20" s="128"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
         <v>79</v>
@@ -15502,17 +15502,17 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="128">
+      <c r="P20" s="129">
         <v>45318</v>
       </c>
-      <c r="Q20" s="128"/>
-      <c r="R20" s="128"/>
+      <c r="Q20" s="129"/>
+      <c r="R20" s="129"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="131">
+      <c r="T20" s="128">
         <v>137</v>
       </c>
-      <c r="U20" s="131"/>
-      <c r="V20" s="131"/>
+      <c r="U20" s="128"/>
+      <c r="V20" s="128"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10" t="str">
@@ -15543,11 +15543,11 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="122"/>
-      <c r="G21" s="136" t="s">
+      <c r="G21" s="135" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="128"/>
-      <c r="I21" s="128"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10" t="s">
         <v>48</v>
@@ -15556,17 +15556,17 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="128">
+      <c r="P21" s="129">
         <v>45317</v>
       </c>
-      <c r="Q21" s="128"/>
-      <c r="R21" s="128"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="131">
+      <c r="T21" s="128">
         <v>138</v>
       </c>
-      <c r="U21" s="131"/>
-      <c r="V21" s="131"/>
+      <c r="U21" s="128"/>
+      <c r="V21" s="128"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10" t="str">
@@ -15597,11 +15597,11 @@
       <c r="C22" s="121"/>
       <c r="D22" s="121"/>
       <c r="E22" s="122"/>
-      <c r="G22" s="136" t="s">
+      <c r="G22" s="135" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="128"/>
-      <c r="I22" s="128"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
         <v>117</v>
@@ -15610,17 +15610,17 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="128">
+      <c r="P22" s="129">
         <v>45316</v>
       </c>
-      <c r="Q22" s="128"/>
-      <c r="R22" s="128"/>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="129"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="131">
+      <c r="T22" s="128">
         <v>139</v>
       </c>
-      <c r="U22" s="131"/>
-      <c r="V22" s="131"/>
+      <c r="U22" s="128"/>
+      <c r="V22" s="128"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10" t="str">
@@ -15651,11 +15651,11 @@
       <c r="C23" s="121"/>
       <c r="D23" s="121"/>
       <c r="E23" s="122"/>
-      <c r="G23" s="136" t="s">
+      <c r="G23" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
         <v>12</v>
@@ -15664,17 +15664,17 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="128">
+      <c r="P23" s="129">
         <v>45315</v>
       </c>
-      <c r="Q23" s="128"/>
-      <c r="R23" s="128"/>
+      <c r="Q23" s="129"/>
+      <c r="R23" s="129"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="131">
+      <c r="T23" s="128">
         <v>140</v>
       </c>
-      <c r="U23" s="131"/>
-      <c r="V23" s="131"/>
+      <c r="U23" s="128"/>
+      <c r="V23" s="128"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10" t="str">
@@ -15707,11 +15707,11 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="122"/>
-      <c r="G24" s="136" t="s">
+      <c r="G24" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
         <v>84</v>
@@ -15720,17 +15720,17 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="128">
+      <c r="P24" s="129">
         <v>45314</v>
       </c>
-      <c r="Q24" s="128"/>
-      <c r="R24" s="128"/>
+      <c r="Q24" s="129"/>
+      <c r="R24" s="129"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="131">
+      <c r="T24" s="128">
         <v>141</v>
       </c>
-      <c r="U24" s="131"/>
-      <c r="V24" s="131"/>
+      <c r="U24" s="128"/>
+      <c r="V24" s="128"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="str">
@@ -15761,11 +15761,11 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="122"/>
-      <c r="G25" s="136" t="s">
+      <c r="G25" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="128"/>
-      <c r="I25" s="128"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10" t="s">
         <v>69</v>
@@ -15774,17 +15774,17 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="128">
+      <c r="P25" s="129">
         <v>45313</v>
       </c>
-      <c r="Q25" s="128"/>
-      <c r="R25" s="128"/>
+      <c r="Q25" s="129"/>
+      <c r="R25" s="129"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="131">
+      <c r="T25" s="128">
         <v>142</v>
       </c>
-      <c r="U25" s="131"/>
-      <c r="V25" s="131"/>
+      <c r="U25" s="128"/>
+      <c r="V25" s="128"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10" t="str">
@@ -15815,11 +15815,11 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="122"/>
-      <c r="G26" s="136" t="s">
+      <c r="G26" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="128"/>
-      <c r="I26" s="128"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="s">
         <v>70</v>
@@ -15828,17 +15828,17 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="128">
+      <c r="P26" s="129">
         <v>45312</v>
       </c>
-      <c r="Q26" s="128"/>
-      <c r="R26" s="128"/>
+      <c r="Q26" s="129"/>
+      <c r="R26" s="129"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="131">
+      <c r="T26" s="128">
         <v>143</v>
       </c>
-      <c r="U26" s="131"/>
-      <c r="V26" s="131"/>
+      <c r="U26" s="128"/>
+      <c r="V26" s="128"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10" t="str">
@@ -15869,11 +15869,11 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="122"/>
-      <c r="G27" s="136" t="s">
+      <c r="G27" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10" t="s">
         <v>71</v>
@@ -15882,17 +15882,17 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="128">
+      <c r="P27" s="129">
         <v>45311</v>
       </c>
-      <c r="Q27" s="128"/>
-      <c r="R27" s="128"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="129"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="131">
+      <c r="T27" s="128">
         <v>144</v>
       </c>
-      <c r="U27" s="131"/>
-      <c r="V27" s="131"/>
+      <c r="U27" s="128"/>
+      <c r="V27" s="128"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10" t="str">
@@ -15923,11 +15923,11 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="122"/>
-      <c r="G28" s="136" t="s">
+      <c r="G28" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="128"/>
-      <c r="I28" s="128"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10" t="s">
         <v>72</v>
@@ -15936,17 +15936,17 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="128">
+      <c r="P28" s="129">
         <v>45310</v>
       </c>
-      <c r="Q28" s="128"/>
-      <c r="R28" s="128"/>
+      <c r="Q28" s="129"/>
+      <c r="R28" s="129"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="131">
+      <c r="T28" s="128">
         <v>145</v>
       </c>
-      <c r="U28" s="131"/>
-      <c r="V28" s="131"/>
+      <c r="U28" s="128"/>
+      <c r="V28" s="128"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10" t="str">
@@ -15977,11 +15977,11 @@
       <c r="C29" s="121"/>
       <c r="D29" s="121"/>
       <c r="E29" s="122"/>
-      <c r="G29" s="136" t="s">
+      <c r="G29" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10" t="s">
         <v>73</v>
@@ -15990,17 +15990,17 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="128">
+      <c r="P29" s="129">
         <v>45309</v>
       </c>
-      <c r="Q29" s="128"/>
-      <c r="R29" s="128"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="131">
+      <c r="T29" s="128">
         <v>146</v>
       </c>
-      <c r="U29" s="131"/>
-      <c r="V29" s="131"/>
+      <c r="U29" s="128"/>
+      <c r="V29" s="128"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10" t="str">
@@ -16031,11 +16031,11 @@
       <c r="C30" s="121"/>
       <c r="D30" s="121"/>
       <c r="E30" s="122"/>
-      <c r="G30" s="135" t="s">
+      <c r="G30" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="129"/>
-      <c r="I30" s="129"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>74</v>
@@ -16044,17 +16044,17 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="129">
+      <c r="P30" s="131">
         <v>45308</v>
       </c>
-      <c r="Q30" s="129"/>
-      <c r="R30" s="129"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
       <c r="S30" s="2"/>
-      <c r="T30" s="132">
+      <c r="T30" s="130">
         <v>147</v>
       </c>
-      <c r="U30" s="132"/>
-      <c r="V30" s="132"/>
+      <c r="U30" s="130"/>
+      <c r="V30" s="130"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2" t="str">
@@ -16082,27 +16082,64 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="T30:V30"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
@@ -16119,64 +16156,27 @@
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="T30:V30"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="T17:V17"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="T19:V19"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="T23:V23"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="T25:V25"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dashboard for group transactions chart image is corrected
</commit_message>
<xml_diff>
--- a/docs/Mockups.xlsx
+++ b/docs/Mockups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="14" r:id="rId1"/>
@@ -1514,14 +1514,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1529,13 +1529,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1544,20 +1538,29 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1566,9 +1569,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1584,6 +1584,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1604,15 +1616,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1621,9 +1624,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1724,17 +1724,17 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>217967</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>10711</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9952</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1747,8 +1747,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1771650" y="1133476"/>
-          <a:ext cx="9476267" cy="3543300"/>
+          <a:off x="1771650" y="1133475"/>
+          <a:ext cx="8497486" cy="3057952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3143,12 +3143,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -3503,6 +3503,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="B30:E30"/>
@@ -3519,18 +3531,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3628,12 +3628,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -3716,11 +3716,11 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="129">
+      <c r="L8" s="128">
         <v>45336</v>
       </c>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
+      <c r="M8" s="128"/>
+      <c r="N8" s="128"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
         <v>127</v>
@@ -3770,11 +3770,11 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="129">
+      <c r="L9" s="128">
         <v>45324</v>
       </c>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
         <v>128</v>
@@ -3826,11 +3826,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="129">
+      <c r="L10" s="128">
         <v>45241</v>
       </c>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
       <c r="O10" s="10"/>
       <c r="P10" s="9" t="s">
         <v>127</v>
@@ -3880,11 +3880,11 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="129">
+      <c r="L11" s="128">
         <v>45281</v>
       </c>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
         <v>129</v>
@@ -3934,11 +3934,11 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="129">
+      <c r="L12" s="128">
         <v>45220</v>
       </c>
-      <c r="M12" s="129"/>
-      <c r="N12" s="129"/>
+      <c r="M12" s="128"/>
+      <c r="N12" s="128"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
         <v>130</v>
@@ -4737,6 +4737,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -4753,21 +4768,6 @@
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4882,12 +4882,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -5462,6 +5462,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B24:E24"/>
@@ -5478,17 +5489,6 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5586,25 +5586,25 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="N5" s="138" t="s">
+      <c r="N5" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="O5" s="139"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="140"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="141"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121" t="s">
@@ -5680,17 +5680,17 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="129">
+      <c r="K8" s="128">
         <v>45353</v>
       </c>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="128">
+      <c r="O8" s="131">
         <v>10</v>
       </c>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="128"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10" t="s">
         <v>127</v>
@@ -5706,9 +5706,9 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
       <c r="AB8" s="10"/>
-      <c r="AC8" s="141"/>
-      <c r="AD8" s="141"/>
-      <c r="AE8" s="141"/>
+      <c r="AC8" s="138"/>
+      <c r="AD8" s="138"/>
+      <c r="AE8" s="138"/>
       <c r="AF8" s="86"/>
       <c r="AG8" s="10" t="s">
         <v>175</v>
@@ -5736,17 +5736,17 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="129">
+      <c r="K9" s="128">
         <v>45353</v>
       </c>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="128">
+      <c r="O9" s="131">
         <v>10</v>
       </c>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="128"/>
+      <c r="P9" s="131"/>
+      <c r="Q9" s="131"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10" t="s">
         <v>127</v>
@@ -5762,9 +5762,9 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
-      <c r="AC9" s="141"/>
-      <c r="AD9" s="141"/>
-      <c r="AE9" s="141"/>
+      <c r="AC9" s="138"/>
+      <c r="AD9" s="138"/>
+      <c r="AE9" s="138"/>
       <c r="AF9" s="86"/>
       <c r="AG9" s="10" t="s">
         <v>175</v>
@@ -5788,13 +5788,13 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="128"/>
-      <c r="Q10" s="128"/>
+      <c r="O10" s="131"/>
+      <c r="P10" s="131"/>
+      <c r="Q10" s="131"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5806,9 +5806,9 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
-      <c r="AC10" s="141"/>
-      <c r="AD10" s="141"/>
-      <c r="AE10" s="141"/>
+      <c r="AC10" s="138"/>
+      <c r="AD10" s="138"/>
+      <c r="AE10" s="138"/>
       <c r="AF10" s="86"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="86"/>
@@ -5834,17 +5834,17 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="129">
+      <c r="K11" s="128">
         <v>45354</v>
       </c>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="128">
+      <c r="O11" s="131">
         <v>5</v>
       </c>
-      <c r="P11" s="128"/>
-      <c r="Q11" s="128"/>
+      <c r="P11" s="131"/>
+      <c r="Q11" s="131"/>
       <c r="R11" s="10"/>
       <c r="S11" s="9" t="s">
         <v>130</v>
@@ -5860,9 +5860,9 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
-      <c r="AC11" s="141"/>
-      <c r="AD11" s="141"/>
-      <c r="AE11" s="141"/>
+      <c r="AC11" s="138"/>
+      <c r="AD11" s="138"/>
+      <c r="AE11" s="138"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="9" t="s">
         <v>176</v>
@@ -5888,17 +5888,17 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="129">
+      <c r="K12" s="128">
         <v>45355</v>
       </c>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="128">
+      <c r="O12" s="131">
         <v>10</v>
       </c>
-      <c r="P12" s="128"/>
-      <c r="Q12" s="128"/>
+      <c r="P12" s="131"/>
+      <c r="Q12" s="131"/>
       <c r="R12" s="10"/>
       <c r="S12" s="9" t="s">
         <v>128</v>
@@ -5944,17 +5944,17 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="129">
+      <c r="K13" s="128">
         <v>45356</v>
       </c>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="128">
+      <c r="O13" s="131">
         <v>20</v>
       </c>
-      <c r="P13" s="128"/>
-      <c r="Q13" s="128"/>
+      <c r="P13" s="131"/>
+      <c r="Q13" s="131"/>
       <c r="R13" s="10"/>
       <c r="S13" s="9" t="s">
         <v>129</v>
@@ -6187,26 +6187,26 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="128">
+      <c r="M21" s="131">
         <v>30</v>
       </c>
-      <c r="N21" s="128"/>
-      <c r="O21" s="128"/>
+      <c r="N21" s="131"/>
+      <c r="O21" s="131"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="128">
+      <c r="Q21" s="131">
         <v>35</v>
       </c>
-      <c r="R21" s="128"/>
-      <c r="S21" s="128"/>
-      <c r="T21" s="128"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="128">
+      <c r="V21" s="131">
         <f>M21-Q21</f>
         <v>-5</v>
       </c>
-      <c r="W21" s="128"/>
-      <c r="X21" s="128"/>
-      <c r="Y21" s="128"/>
+      <c r="W21" s="131"/>
+      <c r="X21" s="131"/>
+      <c r="Y21" s="131"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="44"/>
     </row>
@@ -6223,26 +6223,26 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="128">
+      <c r="M22" s="131">
         <v>20</v>
       </c>
-      <c r="N22" s="128"/>
-      <c r="O22" s="128"/>
+      <c r="N22" s="131"/>
+      <c r="O22" s="131"/>
       <c r="P22" s="10"/>
-      <c r="Q22" s="128">
+      <c r="Q22" s="131">
         <v>10</v>
       </c>
-      <c r="R22" s="128"/>
-      <c r="S22" s="128"/>
-      <c r="T22" s="128"/>
+      <c r="R22" s="131"/>
+      <c r="S22" s="131"/>
+      <c r="T22" s="131"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="128">
+      <c r="V22" s="131">
         <f>M22-Q22</f>
         <v>10</v>
       </c>
-      <c r="W22" s="128"/>
-      <c r="X22" s="128"/>
-      <c r="Y22" s="128"/>
+      <c r="W22" s="131"/>
+      <c r="X22" s="131"/>
+      <c r="Y22" s="131"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="44"/>
     </row>
@@ -6259,26 +6259,26 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="128">
+      <c r="M23" s="131">
         <v>5</v>
       </c>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
+      <c r="N23" s="131"/>
+      <c r="O23" s="131"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="128">
+      <c r="Q23" s="131">
         <v>10</v>
       </c>
-      <c r="R23" s="128"/>
-      <c r="S23" s="128"/>
-      <c r="T23" s="128"/>
+      <c r="R23" s="131"/>
+      <c r="S23" s="131"/>
+      <c r="T23" s="131"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="128">
+      <c r="V23" s="131">
         <f>M23-Q23</f>
         <v>-5</v>
       </c>
-      <c r="W23" s="128"/>
-      <c r="X23" s="128"/>
-      <c r="Y23" s="128"/>
+      <c r="W23" s="131"/>
+      <c r="X23" s="131"/>
+      <c r="Y23" s="131"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="44"/>
     </row>
@@ -6295,26 +6295,26 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="128">
+      <c r="M24" s="131">
         <v>10</v>
       </c>
-      <c r="N24" s="128"/>
-      <c r="O24" s="128"/>
+      <c r="N24" s="131"/>
+      <c r="O24" s="131"/>
       <c r="P24" s="10"/>
-      <c r="Q24" s="128">
+      <c r="Q24" s="131">
         <v>10</v>
       </c>
-      <c r="R24" s="128"/>
-      <c r="S24" s="128"/>
-      <c r="T24" s="128"/>
+      <c r="R24" s="131"/>
+      <c r="S24" s="131"/>
+      <c r="T24" s="131"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="128">
+      <c r="V24" s="131">
         <f>M24-Q24</f>
         <v>0</v>
       </c>
-      <c r="W24" s="128"/>
-      <c r="X24" s="128"/>
-      <c r="Y24" s="128"/>
+      <c r="W24" s="131"/>
+      <c r="X24" s="131"/>
+      <c r="Y24" s="131"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="44"/>
     </row>
@@ -6380,36 +6380,15 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="AC11:AE11"/>
-    <mergeCell ref="AC9:AE9"/>
-    <mergeCell ref="AC10:AE10"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V23:Y23"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="Q22:T22"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="Q24:T24"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="M21:O21"/>
@@ -6426,15 +6405,36 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="Q21:T21"/>
-    <mergeCell ref="Q22:T22"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="AC11:AE11"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="AC10:AE10"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="O11:Q11"/>
   </mergeCells>
   <conditionalFormatting sqref="V21:Y24">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -6559,12 +6559,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -7083,6 +7083,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="H8:R8"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -7099,20 +7113,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7517,10 +7517,10 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="44"/>
-      <c r="J46" s="138" t="s">
+      <c r="J46" s="139" t="s">
         <v>54</v>
       </c>
-      <c r="K46" s="140"/>
+      <c r="K46" s="141"/>
       <c r="M46" s="144"/>
       <c r="N46" s="144"/>
       <c r="O46" s="144"/>
@@ -7939,46 +7939,46 @@
       <c r="C5" s="121"/>
       <c r="D5" s="121"/>
       <c r="E5" s="146"/>
-      <c r="G5" s="159" t="s">
+      <c r="G5" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="159"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
-      <c r="AD5" s="159"/>
-      <c r="AE5" s="159"/>
-      <c r="AF5" s="159"/>
-      <c r="AG5" s="159"/>
-      <c r="AH5" s="159"/>
-      <c r="AI5" s="159"/>
-      <c r="AJ5" s="159"/>
-      <c r="AK5" s="159"/>
-      <c r="AL5" s="159"/>
-      <c r="AM5" s="159"/>
-      <c r="AN5" s="159"/>
-      <c r="AO5" s="159"/>
-      <c r="AP5" s="159"/>
-      <c r="AQ5" s="159"/>
-      <c r="AR5" s="159"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147"/>
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="147"/>
+      <c r="AI5" s="147"/>
+      <c r="AJ5" s="147"/>
+      <c r="AK5" s="147"/>
+      <c r="AL5" s="147"/>
+      <c r="AM5" s="147"/>
+      <c r="AN5" s="147"/>
+      <c r="AO5" s="147"/>
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -8095,13 +8095,13 @@
       <c r="C8" s="121"/>
       <c r="D8" s="121"/>
       <c r="E8" s="146"/>
-      <c r="G8" s="156" t="s">
+      <c r="G8" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="157"/>
-      <c r="K8" s="158"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="159"/>
       <c r="L8" s="25" t="s">
         <v>25</v>
       </c>
@@ -8210,13 +8210,13 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="146"/>
-      <c r="G9" s="153" t="s">
+      <c r="G9" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="155"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="150"/>
       <c r="L9" s="24">
         <f t="shared" ref="L9:M12" si="0">SUM(M9:AQ9)</f>
         <v>610</v>
@@ -8324,13 +8324,13 @@
       <c r="C10" s="121"/>
       <c r="D10" s="121"/>
       <c r="E10" s="146"/>
-      <c r="G10" s="153" t="s">
+      <c r="G10" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="155"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="150"/>
       <c r="L10" s="24">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -8380,13 +8380,13 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="146"/>
-      <c r="G11" s="153" t="s">
+      <c r="G11" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="155"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
+      <c r="K11" s="150"/>
       <c r="L11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8432,13 +8432,13 @@
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
       <c r="E12" s="146"/>
-      <c r="G12" s="153" t="s">
+      <c r="G12" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="155"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="150"/>
       <c r="L12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8484,13 +8484,13 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="146"/>
-      <c r="G13" s="153" t="s">
+      <c r="G13" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="155"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="150"/>
       <c r="L13" s="24">
         <v>500</v>
       </c>
@@ -8541,13 +8541,13 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="146"/>
-      <c r="G14" s="153" t="s">
+      <c r="G14" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="155"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="150"/>
       <c r="L14" s="24">
         <f>SUM(M14:AQ14)</f>
         <v>246</v>
@@ -8595,13 +8595,13 @@
       <c r="C15" s="121"/>
       <c r="D15" s="121"/>
       <c r="E15" s="146"/>
-      <c r="G15" s="153" t="s">
+      <c r="G15" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="155"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="149"/>
+      <c r="K15" s="150"/>
       <c r="L15" s="24">
         <f>SUM(M15:AQ15)</f>
         <v>220</v>
@@ -8649,13 +8649,13 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="G16" s="147" t="s">
+      <c r="G16" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="149"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="153"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="11"/>
@@ -8695,13 +8695,13 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="146"/>
-      <c r="G17" s="150" t="s">
+      <c r="G17" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="152"/>
+      <c r="H17" s="155"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="155"/>
+      <c r="K17" s="156"/>
       <c r="L17" s="26">
         <f>SUM(L9:L16)</f>
         <v>1976</v>
@@ -8863,46 +8863,46 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="146"/>
-      <c r="G21" s="159" t="s">
+      <c r="G21" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="159"/>
-      <c r="O21" s="159"/>
-      <c r="P21" s="159"/>
-      <c r="Q21" s="159"/>
-      <c r="R21" s="159"/>
-      <c r="S21" s="159"/>
-      <c r="T21" s="159"/>
-      <c r="U21" s="159"/>
-      <c r="V21" s="159"/>
-      <c r="W21" s="159"/>
-      <c r="X21" s="159"/>
-      <c r="Y21" s="159"/>
-      <c r="Z21" s="159"/>
-      <c r="AA21" s="159"/>
-      <c r="AB21" s="159"/>
-      <c r="AC21" s="159"/>
-      <c r="AD21" s="159"/>
-      <c r="AE21" s="159"/>
-      <c r="AF21" s="159"/>
-      <c r="AG21" s="159"/>
-      <c r="AH21" s="159"/>
-      <c r="AI21" s="159"/>
-      <c r="AJ21" s="159"/>
-      <c r="AK21" s="159"/>
-      <c r="AL21" s="159"/>
-      <c r="AM21" s="159"/>
-      <c r="AN21" s="159"/>
-      <c r="AO21" s="159"/>
-      <c r="AP21" s="159"/>
-      <c r="AQ21" s="159"/>
-      <c r="AR21" s="159"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="147"/>
+      <c r="K21" s="147"/>
+      <c r="L21" s="147"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="147"/>
+      <c r="O21" s="147"/>
+      <c r="P21" s="147"/>
+      <c r="Q21" s="147"/>
+      <c r="R21" s="147"/>
+      <c r="S21" s="147"/>
+      <c r="T21" s="147"/>
+      <c r="U21" s="147"/>
+      <c r="V21" s="147"/>
+      <c r="W21" s="147"/>
+      <c r="X21" s="147"/>
+      <c r="Y21" s="147"/>
+      <c r="Z21" s="147"/>
+      <c r="AA21" s="147"/>
+      <c r="AB21" s="147"/>
+      <c r="AC21" s="147"/>
+      <c r="AD21" s="147"/>
+      <c r="AE21" s="147"/>
+      <c r="AF21" s="147"/>
+      <c r="AG21" s="147"/>
+      <c r="AH21" s="147"/>
+      <c r="AI21" s="147"/>
+      <c r="AJ21" s="147"/>
+      <c r="AK21" s="147"/>
+      <c r="AL21" s="147"/>
+      <c r="AM21" s="147"/>
+      <c r="AN21" s="147"/>
+      <c r="AO21" s="147"/>
+      <c r="AP21" s="147"/>
+      <c r="AQ21" s="147"/>
+      <c r="AR21" s="147"/>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B22" s="121"/>
@@ -9015,13 +9015,13 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="146"/>
-      <c r="G24" s="156" t="s">
+      <c r="G24" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="158"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="158"/>
+      <c r="K24" s="159"/>
       <c r="L24" s="25" t="s">
         <v>25</v>
       </c>
@@ -9127,13 +9127,13 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="146"/>
-      <c r="G25" s="153" t="s">
+      <c r="G25" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="154"/>
-      <c r="I25" s="154"/>
-      <c r="J25" s="154"/>
-      <c r="K25" s="155"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="150"/>
       <c r="L25" s="24">
         <f>SUM(M25:AQ25)</f>
         <v>610</v>
@@ -9241,13 +9241,13 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="146"/>
-      <c r="G26" s="153" t="s">
+      <c r="G26" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="154"/>
-      <c r="I26" s="154"/>
-      <c r="J26" s="154"/>
-      <c r="K26" s="155"/>
+      <c r="H26" s="149"/>
+      <c r="I26" s="149"/>
+      <c r="J26" s="149"/>
+      <c r="K26" s="150"/>
       <c r="L26" s="24">
         <f>SUM(M26:AQ26)</f>
         <v>400</v>
@@ -9297,13 +9297,13 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="146"/>
-      <c r="G27" s="147" t="s">
+      <c r="G27" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="149"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="152"/>
+      <c r="K27" s="153"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="11"/>
@@ -9343,13 +9343,13 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="146"/>
-      <c r="G28" s="150" t="s">
+      <c r="G28" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="151"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="151"/>
-      <c r="K28" s="152"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="26">
         <f>SUM(L25:L27)</f>
         <v>1010</v>
@@ -9507,15 +9507,24 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G21:AR21"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="G5:AR5"/>
     <mergeCell ref="G9:K9"/>
@@ -9532,24 +9541,15 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G21:AR21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:L16">
     <cfRule type="dataBar" priority="2">
@@ -9708,43 +9708,43 @@
       <c r="G5" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="159"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
-      <c r="AD5" s="159"/>
-      <c r="AE5" s="159"/>
-      <c r="AF5" s="159"/>
-      <c r="AG5" s="159"/>
-      <c r="AH5" s="159"/>
-      <c r="AI5" s="159"/>
-      <c r="AJ5" s="159"/>
-      <c r="AK5" s="159"/>
-      <c r="AL5" s="159"/>
-      <c r="AM5" s="159"/>
-      <c r="AN5" s="159"/>
-      <c r="AO5" s="159"/>
-      <c r="AP5" s="159"/>
-      <c r="AQ5" s="159"/>
-      <c r="AR5" s="159"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147"/>
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="147"/>
+      <c r="AI5" s="147"/>
+      <c r="AJ5" s="147"/>
+      <c r="AK5" s="147"/>
+      <c r="AL5" s="147"/>
+      <c r="AM5" s="147"/>
+      <c r="AN5" s="147"/>
+      <c r="AO5" s="147"/>
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" s="121"/>
@@ -9753,11 +9753,11 @@
       <c r="E6" s="146"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="161"/>
       <c r="G7" s="40" t="s">
         <v>28</v>
@@ -10216,23 +10216,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:AR5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:AR5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11216,7 +11216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="AV29" sqref="AV29"/>
     </sheetView>
   </sheetViews>
@@ -11306,24 +11306,24 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="G5" s="120" t="s">
         <v>168</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="125" t="s">
+      <c r="K5" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
@@ -11500,6 +11500,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B31:E31"/>
@@ -11516,20 +11530,6 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:N5">
@@ -11545,8 +11545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11643,12 +11643,12 @@
       <c r="E5" s="122"/>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -11798,14 +11798,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -11818,12 +11816,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11922,12 +11922,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -12846,14 +12846,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -12866,12 +12864,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12983,12 +12983,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -13229,14 +13229,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
@@ -13249,12 +13247,14 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13352,12 +13352,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -13387,11 +13387,11 @@
       <c r="K7" s="68"/>
       <c r="L7" s="74"/>
       <c r="M7" s="74"/>
-      <c r="N7" s="132" t="s">
+      <c r="N7" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="132"/>
-      <c r="P7" s="132"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
       <c r="Q7" s="68"/>
       <c r="R7" s="68" t="s">
         <v>25</v>
@@ -13428,17 +13428,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="129">
+      <c r="N8" s="128">
         <v>45334</v>
       </c>
-      <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
+      <c r="O8" s="128"/>
+      <c r="P8" s="128"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="128">
+      <c r="R8" s="131">
         <v>500</v>
       </c>
-      <c r="S8" s="128"/>
-      <c r="T8" s="128"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="131"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -13460,17 +13460,17 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="129">
+      <c r="N9" s="128">
         <v>45334</v>
       </c>
-      <c r="O9" s="129"/>
-      <c r="P9" s="129"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="128"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="128">
+      <c r="R9" s="131">
         <v>501</v>
       </c>
-      <c r="S9" s="128"/>
-      <c r="T9" s="128"/>
+      <c r="S9" s="131"/>
+      <c r="T9" s="131"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -13492,17 +13492,17 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="129">
+      <c r="N10" s="128">
         <v>45334</v>
       </c>
-      <c r="O10" s="129"/>
-      <c r="P10" s="129"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="128"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="128">
+      <c r="R10" s="131">
         <v>502</v>
       </c>
-      <c r="S10" s="128"/>
-      <c r="T10" s="128"/>
+      <c r="S10" s="131"/>
+      <c r="T10" s="131"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -13524,17 +13524,17 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="129">
+      <c r="N11" s="128">
         <v>45334</v>
       </c>
-      <c r="O11" s="129"/>
-      <c r="P11" s="129"/>
+      <c r="O11" s="128"/>
+      <c r="P11" s="128"/>
       <c r="Q11" s="10"/>
-      <c r="R11" s="128">
+      <c r="R11" s="131">
         <v>503</v>
       </c>
-      <c r="S11" s="128"/>
-      <c r="T11" s="128"/>
+      <c r="S11" s="131"/>
+      <c r="T11" s="131"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -13556,17 +13556,17 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="129">
+      <c r="N12" s="128">
         <v>45334</v>
       </c>
-      <c r="O12" s="129"/>
-      <c r="P12" s="129"/>
+      <c r="O12" s="128"/>
+      <c r="P12" s="128"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="128">
+      <c r="R12" s="131">
         <v>504</v>
       </c>
-      <c r="S12" s="128"/>
-      <c r="T12" s="128"/>
+      <c r="S12" s="131"/>
+      <c r="T12" s="131"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -13588,17 +13588,17 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="129">
+      <c r="N13" s="128">
         <v>45334</v>
       </c>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
+      <c r="O13" s="128"/>
+      <c r="P13" s="128"/>
       <c r="Q13" s="10"/>
-      <c r="R13" s="128">
+      <c r="R13" s="131">
         <v>505</v>
       </c>
-      <c r="S13" s="128"/>
-      <c r="T13" s="128"/>
+      <c r="S13" s="131"/>
+      <c r="T13" s="131"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -13620,17 +13620,17 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="129">
+      <c r="N14" s="128">
         <v>45334</v>
       </c>
-      <c r="O14" s="129"/>
-      <c r="P14" s="129"/>
+      <c r="O14" s="128"/>
+      <c r="P14" s="128"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="128">
+      <c r="R14" s="131">
         <v>506</v>
       </c>
-      <c r="S14" s="128"/>
-      <c r="T14" s="128"/>
+      <c r="S14" s="131"/>
+      <c r="T14" s="131"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -13652,17 +13652,17 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="129">
+      <c r="N15" s="128">
         <v>45334</v>
       </c>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="128">
+      <c r="R15" s="131">
         <v>507</v>
       </c>
-      <c r="S15" s="128"/>
-      <c r="T15" s="128"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
@@ -13684,17 +13684,17 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="129">
+      <c r="N16" s="128">
         <v>45334</v>
       </c>
-      <c r="O16" s="129"/>
-      <c r="P16" s="129"/>
+      <c r="O16" s="128"/>
+      <c r="P16" s="128"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="128">
+      <c r="R16" s="131">
         <v>508</v>
       </c>
-      <c r="S16" s="128"/>
-      <c r="T16" s="128"/>
+      <c r="S16" s="131"/>
+      <c r="T16" s="131"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -13717,17 +13717,17 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="129">
+      <c r="N17" s="128">
         <v>45334</v>
       </c>
-      <c r="O17" s="129"/>
-      <c r="P17" s="129"/>
+      <c r="O17" s="128"/>
+      <c r="P17" s="128"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="128">
+      <c r="R17" s="131">
         <v>509</v>
       </c>
-      <c r="S17" s="128"/>
-      <c r="T17" s="128"/>
+      <c r="S17" s="131"/>
+      <c r="T17" s="131"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -13749,17 +13749,17 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="129">
+      <c r="N18" s="128">
         <v>45334</v>
       </c>
-      <c r="O18" s="129"/>
-      <c r="P18" s="129"/>
+      <c r="O18" s="128"/>
+      <c r="P18" s="128"/>
       <c r="Q18" s="10"/>
-      <c r="R18" s="128">
+      <c r="R18" s="131">
         <v>510</v>
       </c>
-      <c r="S18" s="128"/>
-      <c r="T18" s="128"/>
+      <c r="S18" s="131"/>
+      <c r="T18" s="131"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
@@ -13781,17 +13781,17 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="129">
+      <c r="N19" s="128">
         <v>45334</v>
       </c>
-      <c r="O19" s="129"/>
-      <c r="P19" s="129"/>
+      <c r="O19" s="128"/>
+      <c r="P19" s="128"/>
       <c r="Q19" s="10"/>
-      <c r="R19" s="128">
+      <c r="R19" s="131">
         <v>511</v>
       </c>
-      <c r="S19" s="128"/>
-      <c r="T19" s="128"/>
+      <c r="S19" s="131"/>
+      <c r="T19" s="131"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -13813,17 +13813,17 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="129">
+      <c r="N20" s="128">
         <v>45334</v>
       </c>
-      <c r="O20" s="129"/>
-      <c r="P20" s="129"/>
+      <c r="O20" s="128"/>
+      <c r="P20" s="128"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="128">
+      <c r="R20" s="131">
         <v>512</v>
       </c>
-      <c r="S20" s="128"/>
-      <c r="T20" s="128"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
@@ -13845,17 +13845,17 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="129">
+      <c r="N21" s="128">
         <v>45292</v>
       </c>
-      <c r="O21" s="129"/>
-      <c r="P21" s="129"/>
+      <c r="O21" s="128"/>
+      <c r="P21" s="128"/>
       <c r="Q21" s="10"/>
-      <c r="R21" s="128">
+      <c r="R21" s="131">
         <v>513</v>
       </c>
-      <c r="S21" s="128"/>
-      <c r="T21" s="128"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -13877,17 +13877,17 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="129">
+      <c r="N22" s="128">
         <v>45292</v>
       </c>
-      <c r="O22" s="129"/>
-      <c r="P22" s="129"/>
+      <c r="O22" s="128"/>
+      <c r="P22" s="128"/>
       <c r="Q22" s="10"/>
-      <c r="R22" s="128">
+      <c r="R22" s="131">
         <v>514</v>
       </c>
-      <c r="S22" s="128"/>
-      <c r="T22" s="128"/>
+      <c r="S22" s="131"/>
+      <c r="T22" s="131"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
@@ -13909,17 +13909,17 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="129">
+      <c r="N23" s="128">
         <v>45292</v>
       </c>
-      <c r="O23" s="129"/>
-      <c r="P23" s="129"/>
+      <c r="O23" s="128"/>
+      <c r="P23" s="128"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="128">
+      <c r="R23" s="131">
         <v>515</v>
       </c>
-      <c r="S23" s="128"/>
-      <c r="T23" s="128"/>
+      <c r="S23" s="131"/>
+      <c r="T23" s="131"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -13941,17 +13941,17 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="129">
+      <c r="N24" s="128">
         <v>45292</v>
       </c>
-      <c r="O24" s="129"/>
-      <c r="P24" s="129"/>
+      <c r="O24" s="128"/>
+      <c r="P24" s="128"/>
       <c r="Q24" s="10"/>
-      <c r="R24" s="128">
+      <c r="R24" s="131">
         <v>516</v>
       </c>
-      <c r="S24" s="128"/>
-      <c r="T24" s="128"/>
+      <c r="S24" s="131"/>
+      <c r="T24" s="131"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -13973,17 +13973,17 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="129">
+      <c r="N25" s="128">
         <v>45292</v>
       </c>
-      <c r="O25" s="129"/>
-      <c r="P25" s="129"/>
+      <c r="O25" s="128"/>
+      <c r="P25" s="128"/>
       <c r="Q25" s="10"/>
-      <c r="R25" s="128">
+      <c r="R25" s="131">
         <v>517</v>
       </c>
-      <c r="S25" s="128"/>
-      <c r="T25" s="128"/>
+      <c r="S25" s="131"/>
+      <c r="T25" s="131"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -14005,17 +14005,17 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="129">
+      <c r="N26" s="128">
         <v>45292</v>
       </c>
-      <c r="O26" s="129"/>
-      <c r="P26" s="129"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="128"/>
       <c r="Q26" s="10"/>
-      <c r="R26" s="128">
+      <c r="R26" s="131">
         <v>518</v>
       </c>
-      <c r="S26" s="128"/>
-      <c r="T26" s="128"/>
+      <c r="S26" s="131"/>
+      <c r="T26" s="131"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -14037,17 +14037,17 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="129">
+      <c r="N27" s="128">
         <v>45292</v>
       </c>
-      <c r="O27" s="129"/>
-      <c r="P27" s="129"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="128"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="128">
+      <c r="R27" s="131">
         <v>519</v>
       </c>
-      <c r="S27" s="128"/>
-      <c r="T27" s="128"/>
+      <c r="S27" s="131"/>
+      <c r="T27" s="131"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
@@ -14069,17 +14069,17 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="129">
+      <c r="N28" s="128">
         <v>45292</v>
       </c>
-      <c r="O28" s="129"/>
-      <c r="P28" s="129"/>
+      <c r="O28" s="128"/>
+      <c r="P28" s="128"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="128">
+      <c r="R28" s="131">
         <v>520</v>
       </c>
-      <c r="S28" s="128"/>
-      <c r="T28" s="128"/>
+      <c r="S28" s="131"/>
+      <c r="T28" s="131"/>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
@@ -14101,17 +14101,17 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="129">
+      <c r="N29" s="128">
         <v>45292</v>
       </c>
-      <c r="O29" s="129"/>
-      <c r="P29" s="129"/>
+      <c r="O29" s="128"/>
+      <c r="P29" s="128"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="128">
+      <c r="R29" s="131">
         <v>521</v>
       </c>
-      <c r="S29" s="128"/>
-      <c r="T29" s="128"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="131"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
@@ -14133,17 +14133,17 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="131">
+      <c r="N30" s="129">
         <v>45292</v>
       </c>
-      <c r="O30" s="131"/>
-      <c r="P30" s="131"/>
+      <c r="O30" s="129"/>
+      <c r="P30" s="129"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="130">
+      <c r="R30" s="132">
         <v>522</v>
       </c>
-      <c r="S30" s="130"/>
-      <c r="T30" s="130"/>
+      <c r="S30" s="132"/>
+      <c r="T30" s="132"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -14153,6 +14153,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="R26:T26"/>
     <mergeCell ref="N27:P27"/>
     <mergeCell ref="N28:P28"/>
     <mergeCell ref="N29:P29"/>
@@ -14169,63 +14226,6 @@
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14337,12 +14337,12 @@
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" s="121"/>
@@ -14631,6 +14631,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H12:J12"/>
@@ -14647,18 +14659,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14758,12 +14758,12 @@
       <c r="E4" s="122"/>
     </row>
     <row r="5" spans="2:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="125"/>
       <c r="F5" t="s">
         <v>95</v>
       </c>
@@ -14838,11 +14838,11 @@
       <c r="C8" s="126"/>
       <c r="D8" s="126"/>
       <c r="E8" s="127"/>
-      <c r="G8" s="135" t="s">
+      <c r="G8" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10" t="s">
         <v>12</v>
@@ -14851,17 +14851,17 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="129">
+      <c r="P8" s="128">
         <v>45330</v>
       </c>
-      <c r="Q8" s="129"/>
-      <c r="R8" s="129"/>
+      <c r="Q8" s="128"/>
+      <c r="R8" s="128"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="128">
+      <c r="T8" s="131">
         <v>125</v>
       </c>
-      <c r="U8" s="128"/>
-      <c r="V8" s="128"/>
+      <c r="U8" s="131"/>
+      <c r="V8" s="131"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10" t="str">
@@ -14892,11 +14892,11 @@
       <c r="C9" s="121"/>
       <c r="D9" s="121"/>
       <c r="E9" s="122"/>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>84</v>
@@ -14905,17 +14905,17 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="129">
+      <c r="P9" s="128">
         <v>45329</v>
       </c>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
+      <c r="Q9" s="128"/>
+      <c r="R9" s="128"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="128">
+      <c r="T9" s="131">
         <v>120</v>
       </c>
-      <c r="U9" s="128"/>
-      <c r="V9" s="128"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="131"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10" t="str">
@@ -14948,11 +14948,11 @@
       <c r="C10" s="126"/>
       <c r="D10" s="126"/>
       <c r="E10" s="127"/>
-      <c r="G10" s="135" t="s">
+      <c r="G10" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="129"/>
-      <c r="I10" s="129"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
         <v>69</v>
@@ -14961,17 +14961,17 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="129">
+      <c r="P10" s="128">
         <v>45328</v>
       </c>
-      <c r="Q10" s="129"/>
-      <c r="R10" s="129"/>
+      <c r="Q10" s="128"/>
+      <c r="R10" s="128"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="128">
+      <c r="T10" s="131">
         <v>127</v>
       </c>
-      <c r="U10" s="128"/>
-      <c r="V10" s="128"/>
+      <c r="U10" s="131"/>
+      <c r="V10" s="131"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10" t="str">
@@ -15002,11 +15002,11 @@
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
       <c r="E11" s="122"/>
-      <c r="G11" s="135" t="s">
+      <c r="G11" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
         <v>70</v>
@@ -15015,17 +15015,17 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="129">
+      <c r="P11" s="128">
         <v>45327</v>
       </c>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
+      <c r="Q11" s="128"/>
+      <c r="R11" s="128"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="128">
+      <c r="T11" s="131">
         <v>128</v>
       </c>
-      <c r="U11" s="128"/>
-      <c r="V11" s="128"/>
+      <c r="U11" s="131"/>
+      <c r="V11" s="131"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10" t="str">
@@ -15056,11 +15056,11 @@
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
       <c r="E12" s="127"/>
-      <c r="G12" s="135" t="s">
+      <c r="G12" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="129"/>
-      <c r="I12" s="129"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10" t="s">
         <v>71</v>
@@ -15069,17 +15069,17 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="129">
+      <c r="P12" s="128">
         <v>45326</v>
       </c>
-      <c r="Q12" s="129"/>
-      <c r="R12" s="129"/>
+      <c r="Q12" s="128"/>
+      <c r="R12" s="128"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="128">
+      <c r="T12" s="131">
         <v>129</v>
       </c>
-      <c r="U12" s="128"/>
-      <c r="V12" s="128"/>
+      <c r="U12" s="131"/>
+      <c r="V12" s="131"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10" t="str">
@@ -15110,11 +15110,11 @@
       <c r="C13" s="121"/>
       <c r="D13" s="121"/>
       <c r="E13" s="122"/>
-      <c r="G13" s="135" t="s">
+      <c r="G13" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
         <v>72</v>
@@ -15123,17 +15123,17 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="129">
+      <c r="P13" s="128">
         <v>45325</v>
       </c>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
+      <c r="Q13" s="128"/>
+      <c r="R13" s="128"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="128">
+      <c r="T13" s="131">
         <v>130</v>
       </c>
-      <c r="U13" s="128"/>
-      <c r="V13" s="128"/>
+      <c r="U13" s="131"/>
+      <c r="V13" s="131"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10" t="str">
@@ -15164,11 +15164,11 @@
       <c r="C14" s="121"/>
       <c r="D14" s="121"/>
       <c r="E14" s="122"/>
-      <c r="G14" s="135" t="s">
+      <c r="G14" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
         <v>73</v>
@@ -15177,17 +15177,17 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="129">
+      <c r="P14" s="128">
         <v>45324</v>
       </c>
-      <c r="Q14" s="129"/>
-      <c r="R14" s="129"/>
+      <c r="Q14" s="128"/>
+      <c r="R14" s="128"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="128">
+      <c r="T14" s="131">
         <v>131</v>
       </c>
-      <c r="U14" s="128"/>
-      <c r="V14" s="128"/>
+      <c r="U14" s="131"/>
+      <c r="V14" s="131"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10" t="str">
@@ -15218,11 +15218,11 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="63"/>
-      <c r="G15" s="135" t="s">
+      <c r="G15" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
         <v>74</v>
@@ -15231,17 +15231,17 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="129">
+      <c r="P15" s="128">
         <v>45323</v>
       </c>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
+      <c r="Q15" s="128"/>
+      <c r="R15" s="128"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="128">
+      <c r="T15" s="131">
         <v>132</v>
       </c>
-      <c r="U15" s="128"/>
-      <c r="V15" s="128"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="131"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10" t="str">
@@ -15272,11 +15272,11 @@
       <c r="C16" s="121"/>
       <c r="D16" s="121"/>
       <c r="E16" s="122"/>
-      <c r="G16" s="135" t="s">
+      <c r="G16" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="129"/>
-      <c r="I16" s="129"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
         <v>75</v>
@@ -15285,17 +15285,17 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="129">
+      <c r="P16" s="128">
         <v>45322</v>
       </c>
-      <c r="Q16" s="129"/>
-      <c r="R16" s="129"/>
+      <c r="Q16" s="128"/>
+      <c r="R16" s="128"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="128">
+      <c r="T16" s="131">
         <v>133</v>
       </c>
-      <c r="U16" s="128"/>
-      <c r="V16" s="128"/>
+      <c r="U16" s="131"/>
+      <c r="V16" s="131"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10" t="str">
@@ -15327,11 +15327,11 @@
       <c r="C17" s="121"/>
       <c r="D17" s="121"/>
       <c r="E17" s="122"/>
-      <c r="G17" s="135" t="s">
+      <c r="G17" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
         <v>76</v>
@@ -15340,17 +15340,17 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="129">
+      <c r="P17" s="128">
         <v>45321</v>
       </c>
-      <c r="Q17" s="129"/>
-      <c r="R17" s="129"/>
+      <c r="Q17" s="128"/>
+      <c r="R17" s="128"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="128">
+      <c r="T17" s="131">
         <v>134</v>
       </c>
-      <c r="U17" s="128"/>
-      <c r="V17" s="128"/>
+      <c r="U17" s="131"/>
+      <c r="V17" s="131"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10" t="str">
@@ -15381,11 +15381,11 @@
       <c r="C18" s="121"/>
       <c r="D18" s="121"/>
       <c r="E18" s="122"/>
-      <c r="G18" s="135" t="s">
+      <c r="G18" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="129"/>
-      <c r="I18" s="129"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
         <v>77</v>
@@ -15394,17 +15394,17 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="129">
+      <c r="P18" s="128">
         <v>45320</v>
       </c>
-      <c r="Q18" s="129"/>
-      <c r="R18" s="129"/>
+      <c r="Q18" s="128"/>
+      <c r="R18" s="128"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="128">
+      <c r="T18" s="131">
         <v>135</v>
       </c>
-      <c r="U18" s="128"/>
-      <c r="V18" s="128"/>
+      <c r="U18" s="131"/>
+      <c r="V18" s="131"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10" t="str">
@@ -15435,11 +15435,11 @@
       <c r="C19" s="121"/>
       <c r="D19" s="121"/>
       <c r="E19" s="122"/>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="129"/>
-      <c r="I19" s="129"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
         <v>78</v>
@@ -15448,17 +15448,17 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="129">
+      <c r="P19" s="128">
         <v>45319</v>
       </c>
-      <c r="Q19" s="129"/>
-      <c r="R19" s="129"/>
+      <c r="Q19" s="128"/>
+      <c r="R19" s="128"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="128">
+      <c r="T19" s="131">
         <v>136</v>
       </c>
-      <c r="U19" s="128"/>
-      <c r="V19" s="128"/>
+      <c r="U19" s="131"/>
+      <c r="V19" s="131"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10" t="str">
@@ -15489,11 +15489,11 @@
       <c r="C20" s="121"/>
       <c r="D20" s="121"/>
       <c r="E20" s="122"/>
-      <c r="G20" s="135" t="s">
+      <c r="G20" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
         <v>79</v>
@@ -15502,17 +15502,17 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="129">
+      <c r="P20" s="128">
         <v>45318</v>
       </c>
-      <c r="Q20" s="129"/>
-      <c r="R20" s="129"/>
+      <c r="Q20" s="128"/>
+      <c r="R20" s="128"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="128">
+      <c r="T20" s="131">
         <v>137</v>
       </c>
-      <c r="U20" s="128"/>
-      <c r="V20" s="128"/>
+      <c r="U20" s="131"/>
+      <c r="V20" s="131"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10" t="str">
@@ -15543,11 +15543,11 @@
       <c r="C21" s="121"/>
       <c r="D21" s="121"/>
       <c r="E21" s="122"/>
-      <c r="G21" s="135" t="s">
+      <c r="G21" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="129"/>
-      <c r="I21" s="129"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10" t="s">
         <v>48</v>
@@ -15556,17 +15556,17 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="129">
+      <c r="P21" s="128">
         <v>45317</v>
       </c>
-      <c r="Q21" s="129"/>
-      <c r="R21" s="129"/>
+      <c r="Q21" s="128"/>
+      <c r="R21" s="128"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="128">
+      <c r="T21" s="131">
         <v>138</v>
       </c>
-      <c r="U21" s="128"/>
-      <c r="V21" s="128"/>
+      <c r="U21" s="131"/>
+      <c r="V21" s="131"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10" t="str">
@@ -15597,11 +15597,11 @@
       <c r="C22" s="121"/>
       <c r="D22" s="121"/>
       <c r="E22" s="122"/>
-      <c r="G22" s="135" t="s">
+      <c r="G22" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
         <v>117</v>
@@ -15610,17 +15610,17 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="129">
+      <c r="P22" s="128">
         <v>45316</v>
       </c>
-      <c r="Q22" s="129"/>
-      <c r="R22" s="129"/>
+      <c r="Q22" s="128"/>
+      <c r="R22" s="128"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="128">
+      <c r="T22" s="131">
         <v>139</v>
       </c>
-      <c r="U22" s="128"/>
-      <c r="V22" s="128"/>
+      <c r="U22" s="131"/>
+      <c r="V22" s="131"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10" t="str">
@@ -15651,11 +15651,11 @@
       <c r="C23" s="121"/>
       <c r="D23" s="121"/>
       <c r="E23" s="122"/>
-      <c r="G23" s="135" t="s">
+      <c r="G23" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="129"/>
-      <c r="I23" s="129"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
         <v>12</v>
@@ -15664,17 +15664,17 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="129">
+      <c r="P23" s="128">
         <v>45315</v>
       </c>
-      <c r="Q23" s="129"/>
-      <c r="R23" s="129"/>
+      <c r="Q23" s="128"/>
+      <c r="R23" s="128"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="128">
+      <c r="T23" s="131">
         <v>140</v>
       </c>
-      <c r="U23" s="128"/>
-      <c r="V23" s="128"/>
+      <c r="U23" s="131"/>
+      <c r="V23" s="131"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10" t="str">
@@ -15707,11 +15707,11 @@
       <c r="C24" s="121"/>
       <c r="D24" s="121"/>
       <c r="E24" s="122"/>
-      <c r="G24" s="135" t="s">
+      <c r="G24" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="129"/>
-      <c r="I24" s="129"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
         <v>84</v>
@@ -15720,17 +15720,17 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="129">
+      <c r="P24" s="128">
         <v>45314</v>
       </c>
-      <c r="Q24" s="129"/>
-      <c r="R24" s="129"/>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="128"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="128">
+      <c r="T24" s="131">
         <v>141</v>
       </c>
-      <c r="U24" s="128"/>
-      <c r="V24" s="128"/>
+      <c r="U24" s="131"/>
+      <c r="V24" s="131"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10" t="str">
@@ -15761,11 +15761,11 @@
       <c r="C25" s="121"/>
       <c r="D25" s="121"/>
       <c r="E25" s="122"/>
-      <c r="G25" s="135" t="s">
+      <c r="G25" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="129"/>
-      <c r="I25" s="129"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10" t="s">
         <v>69</v>
@@ -15774,17 +15774,17 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="129">
+      <c r="P25" s="128">
         <v>45313</v>
       </c>
-      <c r="Q25" s="129"/>
-      <c r="R25" s="129"/>
+      <c r="Q25" s="128"/>
+      <c r="R25" s="128"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="128">
+      <c r="T25" s="131">
         <v>142</v>
       </c>
-      <c r="U25" s="128"/>
-      <c r="V25" s="128"/>
+      <c r="U25" s="131"/>
+      <c r="V25" s="131"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10" t="str">
@@ -15815,11 +15815,11 @@
       <c r="C26" s="121"/>
       <c r="D26" s="121"/>
       <c r="E26" s="122"/>
-      <c r="G26" s="135" t="s">
+      <c r="G26" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="129"/>
-      <c r="I26" s="129"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="s">
         <v>70</v>
@@ -15828,17 +15828,17 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="129">
+      <c r="P26" s="128">
         <v>45312</v>
       </c>
-      <c r="Q26" s="129"/>
-      <c r="R26" s="129"/>
+      <c r="Q26" s="128"/>
+      <c r="R26" s="128"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="128">
+      <c r="T26" s="131">
         <v>143</v>
       </c>
-      <c r="U26" s="128"/>
-      <c r="V26" s="128"/>
+      <c r="U26" s="131"/>
+      <c r="V26" s="131"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10" t="str">
@@ -15869,11 +15869,11 @@
       <c r="C27" s="121"/>
       <c r="D27" s="121"/>
       <c r="E27" s="122"/>
-      <c r="G27" s="135" t="s">
+      <c r="G27" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10" t="s">
         <v>71</v>
@@ -15882,17 +15882,17 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="129">
+      <c r="P27" s="128">
         <v>45311</v>
       </c>
-      <c r="Q27" s="129"/>
-      <c r="R27" s="129"/>
+      <c r="Q27" s="128"/>
+      <c r="R27" s="128"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="128">
+      <c r="T27" s="131">
         <v>144</v>
       </c>
-      <c r="U27" s="128"/>
-      <c r="V27" s="128"/>
+      <c r="U27" s="131"/>
+      <c r="V27" s="131"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10" t="str">
@@ -15923,11 +15923,11 @@
       <c r="C28" s="121"/>
       <c r="D28" s="121"/>
       <c r="E28" s="122"/>
-      <c r="G28" s="135" t="s">
+      <c r="G28" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="129"/>
-      <c r="I28" s="129"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10" t="s">
         <v>72</v>
@@ -15936,17 +15936,17 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="129">
+      <c r="P28" s="128">
         <v>45310</v>
       </c>
-      <c r="Q28" s="129"/>
-      <c r="R28" s="129"/>
+      <c r="Q28" s="128"/>
+      <c r="R28" s="128"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="128">
+      <c r="T28" s="131">
         <v>145</v>
       </c>
-      <c r="U28" s="128"/>
-      <c r="V28" s="128"/>
+      <c r="U28" s="131"/>
+      <c r="V28" s="131"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10" t="str">
@@ -15977,11 +15977,11 @@
       <c r="C29" s="121"/>
       <c r="D29" s="121"/>
       <c r="E29" s="122"/>
-      <c r="G29" s="135" t="s">
+      <c r="G29" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="129"/>
-      <c r="I29" s="129"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10" t="s">
         <v>73</v>
@@ -15990,17 +15990,17 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="129">
+      <c r="P29" s="128">
         <v>45309</v>
       </c>
-      <c r="Q29" s="129"/>
-      <c r="R29" s="129"/>
+      <c r="Q29" s="128"/>
+      <c r="R29" s="128"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="128">
+      <c r="T29" s="131">
         <v>146</v>
       </c>
-      <c r="U29" s="128"/>
-      <c r="V29" s="128"/>
+      <c r="U29" s="131"/>
+      <c r="V29" s="131"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10" t="str">
@@ -16031,11 +16031,11 @@
       <c r="C30" s="121"/>
       <c r="D30" s="121"/>
       <c r="E30" s="122"/>
-      <c r="G30" s="136" t="s">
+      <c r="G30" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>74</v>
@@ -16044,17 +16044,17 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="131">
+      <c r="P30" s="129">
         <v>45308</v>
       </c>
-      <c r="Q30" s="131"/>
-      <c r="R30" s="131"/>
+      <c r="Q30" s="129"/>
+      <c r="R30" s="129"/>
       <c r="S30" s="2"/>
-      <c r="T30" s="130">
+      <c r="T30" s="132">
         <v>147</v>
       </c>
-      <c r="U30" s="130"/>
-      <c r="V30" s="130"/>
+      <c r="U30" s="132"/>
+      <c r="V30" s="132"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2" t="str">
@@ -16082,43 +16082,48 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="T19:V19"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="T23:V23"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="T25:V25"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="T17:V17"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="T8:V8"/>
     <mergeCell ref="T9:V9"/>
@@ -16135,48 +16140,43 @@
     <mergeCell ref="T30:V30"/>
     <mergeCell ref="P8:R8"/>
     <mergeCell ref="P9:R9"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P29:R29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>